<commit_message>
Updated with latest Logical network drawing
</commit_message>
<xml_diff>
--- a/data/sample_switch_configs/PowerEdge-R/Solution-Workbook.xlsx
+++ b/data/sample_switch_configs/PowerEdge-R/Solution-Workbook.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JetStream-10.0\April-25-2017\JetStream\data\sample_switch_configs\PowerEdge-R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RANDY_perryman\Documents\GitHub\dell-esg\JetPack\data\sample_switch_configs\PowerEdge-R\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" tabRatio="888" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" tabRatio="888" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -6331,6 +6331,45 @@
     <xf numFmtId="0" fontId="0" fillId="97" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="39" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="40" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="41" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="37" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="6" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="38" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="19" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="20" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="21" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="34" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="35" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="26" borderId="35" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="36" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="26" borderId="19" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6370,60 +6409,145 @@
     <xf numFmtId="0" fontId="43" fillId="27" borderId="33" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="19" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="20" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="21" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="34" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="35" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="26" borderId="35" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="36" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="39" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="40" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="41" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="37" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="6" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="38" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="41" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="41" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="41" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="27" borderId="31" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="27" borderId="32" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="27" borderId="33" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="19" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="20" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="21" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="22" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="24" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="8" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="25" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="82" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="77" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="83" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="58" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="12" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="59" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="41" borderId="39" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="60" fillId="41" borderId="40" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="53" fillId="41" borderId="40" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -6437,10 +6561,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="58" xfId="1629" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="58" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -6458,126 +6578,6 @@
     <xf numFmtId="0" fontId="60" fillId="41" borderId="37" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="60" fillId="41" borderId="6" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="53" fillId="41" borderId="6" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="41" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="41" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="41" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="12" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="59" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="82" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="77" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="83" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="27" borderId="31" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="27" borderId="32" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="27" borderId="33" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="19" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="20" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="21" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="22" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="24" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="8" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="25" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6610,60 +6610,72 @@
     <xf numFmtId="0" fontId="49" fillId="25" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="37" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="33" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="38" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="33" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="38" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="37" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="38" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="38" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="38" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="36" fillId="32" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6685,29 +6697,8 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="38" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="38" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="38" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="36" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="36" fillId="36" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -6716,6 +6707,15 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="33" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="38" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10348,15 +10348,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>336550</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>45</xdr:row>
-          <xdr:rowOff>6350</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -10453,33 +10453,39 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>84666</xdr:colOff>
+      <xdr:colOff>214312</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>58419</xdr:rowOff>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>501650</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>183895</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>149170</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="84666" y="58419"/>
-          <a:ext cx="10780184" cy="8964676"/>
+          <a:off x="214312" y="100012"/>
+          <a:ext cx="9777412" cy="8631183"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13097,7 +13103,7 @@
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1"/>
@@ -13114,7 +13120,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" ht="19">
+    <row r="2" spans="1:13" ht="18.75">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -13178,7 +13184,7 @@
       <c r="L5" s="8"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1">
+    <row r="6" spans="1:13" ht="15.75" thickBot="1">
       <c r="A6" s="4"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -13193,21 +13199,21 @@
       <c r="L6" s="8"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" ht="15.5">
+    <row r="7" spans="1:13" ht="15.75">
       <c r="A7" s="4"/>
-      <c r="B7" s="198" t="s">
+      <c r="B7" s="211" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="199"/>
-      <c r="D7" s="199"/>
-      <c r="E7" s="199"/>
-      <c r="F7" s="199"/>
-      <c r="G7" s="199"/>
-      <c r="H7" s="199"/>
-      <c r="I7" s="199"/>
-      <c r="J7" s="199"/>
-      <c r="K7" s="199"/>
-      <c r="L7" s="200"/>
+      <c r="C7" s="212"/>
+      <c r="D7" s="212"/>
+      <c r="E7" s="212"/>
+      <c r="F7" s="212"/>
+      <c r="G7" s="212"/>
+      <c r="H7" s="212"/>
+      <c r="I7" s="212"/>
+      <c r="J7" s="212"/>
+      <c r="K7" s="212"/>
+      <c r="L7" s="213"/>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1">
@@ -13293,21 +13299,21 @@
       <c r="L12" s="15"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="15.5">
+    <row r="13" spans="1:13" ht="15.75">
       <c r="A13" s="4"/>
-      <c r="B13" s="201" t="s">
+      <c r="B13" s="214" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="202"/>
-      <c r="D13" s="202"/>
-      <c r="E13" s="202"/>
-      <c r="F13" s="202"/>
-      <c r="G13" s="202"/>
-      <c r="H13" s="202"/>
-      <c r="I13" s="202"/>
-      <c r="J13" s="202"/>
-      <c r="K13" s="202"/>
-      <c r="L13" s="203"/>
+      <c r="C13" s="215"/>
+      <c r="D13" s="215"/>
+      <c r="E13" s="215"/>
+      <c r="F13" s="215"/>
+      <c r="G13" s="215"/>
+      <c r="H13" s="215"/>
+      <c r="I13" s="215"/>
+      <c r="J13" s="215"/>
+      <c r="K13" s="215"/>
+      <c r="L13" s="216"/>
       <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1">
@@ -13393,21 +13399,21 @@
       <c r="L18" s="18"/>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:13" ht="15.5">
+    <row r="19" spans="1:13" ht="15.75">
       <c r="A19" s="4"/>
-      <c r="B19" s="204" t="s">
+      <c r="B19" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="205"/>
-      <c r="D19" s="205"/>
-      <c r="E19" s="205"/>
-      <c r="F19" s="205"/>
-      <c r="G19" s="205"/>
-      <c r="H19" s="205"/>
-      <c r="I19" s="205"/>
-      <c r="J19" s="205"/>
-      <c r="K19" s="205"/>
-      <c r="L19" s="206"/>
+      <c r="C19" s="218"/>
+      <c r="D19" s="218"/>
+      <c r="E19" s="218"/>
+      <c r="F19" s="218"/>
+      <c r="G19" s="218"/>
+      <c r="H19" s="218"/>
+      <c r="I19" s="218"/>
+      <c r="J19" s="218"/>
+      <c r="K19" s="218"/>
+      <c r="L19" s="219"/>
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1">
@@ -13444,7 +13450,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="1:13" ht="15" thickBot="1">
+    <row r="22" spans="1:13" ht="15.75" thickBot="1">
       <c r="A22" s="4"/>
       <c r="B22" s="19" t="s">
         <v>14</v>
@@ -13461,7 +13467,7 @@
       <c r="L22" s="21"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="1:13" ht="15" thickBot="1">
+    <row r="23" spans="1:13" ht="15.75" thickBot="1">
       <c r="A23" s="4"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
@@ -13478,19 +13484,19 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="4"/>
-      <c r="B24" s="207" t="s">
+      <c r="B24" s="220" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="208"/>
-      <c r="D24" s="208"/>
-      <c r="E24" s="208"/>
-      <c r="F24" s="208"/>
-      <c r="G24" s="208"/>
-      <c r="H24" s="208"/>
-      <c r="I24" s="208"/>
-      <c r="J24" s="208"/>
-      <c r="K24" s="208"/>
-      <c r="L24" s="209"/>
+      <c r="C24" s="221"/>
+      <c r="D24" s="221"/>
+      <c r="E24" s="221"/>
+      <c r="F24" s="221"/>
+      <c r="G24" s="221"/>
+      <c r="H24" s="221"/>
+      <c r="I24" s="221"/>
+      <c r="J24" s="221"/>
+      <c r="K24" s="221"/>
+      <c r="L24" s="222"/>
       <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1">
@@ -13612,7 +13618,7 @@
       <c r="L31" s="12"/>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="1:13" ht="15" thickBot="1">
+    <row r="32" spans="1:13" ht="15.75" thickBot="1">
       <c r="A32" s="4"/>
       <c r="B32" s="19" t="s">
         <v>23</v>
@@ -13629,7 +13635,7 @@
       <c r="L32" s="28"/>
       <c r="M32" s="9"/>
     </row>
-    <row r="33" spans="1:13" ht="15" thickBot="1">
+    <row r="33" spans="1:13" ht="15.75" thickBot="1">
       <c r="A33" s="4"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
@@ -13644,112 +13650,112 @@
       <c r="L33" s="29"/>
       <c r="M33" s="9"/>
     </row>
-    <row r="34" spans="1:13" ht="15" thickBot="1">
+    <row r="34" spans="1:13" ht="15.75" thickBot="1">
       <c r="A34" s="4"/>
-      <c r="B34" s="210" t="s">
+      <c r="B34" s="223" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="211"/>
-      <c r="D34" s="211"/>
-      <c r="E34" s="211"/>
-      <c r="F34" s="211"/>
-      <c r="G34" s="211"/>
-      <c r="H34" s="211"/>
-      <c r="I34" s="211"/>
-      <c r="J34" s="211"/>
-      <c r="K34" s="211"/>
-      <c r="L34" s="212"/>
+      <c r="C34" s="224"/>
+      <c r="D34" s="224"/>
+      <c r="E34" s="224"/>
+      <c r="F34" s="224"/>
+      <c r="G34" s="224"/>
+      <c r="H34" s="224"/>
+      <c r="I34" s="224"/>
+      <c r="J34" s="224"/>
+      <c r="K34" s="224"/>
+      <c r="L34" s="225"/>
       <c r="M34" s="9"/>
     </row>
-    <row r="35" spans="1:13" ht="15" thickBot="1">
+    <row r="35" spans="1:13" ht="15.75" thickBot="1">
       <c r="A35" s="4"/>
-      <c r="B35" s="213" t="s">
+      <c r="B35" s="204" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="214"/>
-      <c r="D35" s="215"/>
-      <c r="E35" s="213" t="s">
+      <c r="C35" s="205"/>
+      <c r="D35" s="206"/>
+      <c r="E35" s="204" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="214"/>
-      <c r="G35" s="215"/>
-      <c r="H35" s="213" t="s">
+      <c r="F35" s="205"/>
+      <c r="G35" s="206"/>
+      <c r="H35" s="204" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="214"/>
-      <c r="J35" s="215"/>
-      <c r="K35" s="213" t="s">
+      <c r="I35" s="205"/>
+      <c r="J35" s="206"/>
+      <c r="K35" s="204" t="s">
         <v>28</v>
       </c>
-      <c r="L35" s="215"/>
+      <c r="L35" s="206"/>
       <c r="M35" s="9"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="4"/>
-      <c r="B36" s="216">
+      <c r="B36" s="207">
         <v>1</v>
       </c>
-      <c r="C36" s="217"/>
-      <c r="D36" s="217"/>
-      <c r="E36" s="218"/>
-      <c r="F36" s="217"/>
-      <c r="G36" s="217"/>
-      <c r="H36" s="217"/>
-      <c r="I36" s="217"/>
-      <c r="J36" s="217"/>
-      <c r="K36" s="217"/>
-      <c r="L36" s="219"/>
+      <c r="C36" s="208"/>
+      <c r="D36" s="208"/>
+      <c r="E36" s="209"/>
+      <c r="F36" s="208"/>
+      <c r="G36" s="208"/>
+      <c r="H36" s="208"/>
+      <c r="I36" s="208"/>
+      <c r="J36" s="208"/>
+      <c r="K36" s="208"/>
+      <c r="L36" s="210"/>
       <c r="M36" s="9"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="4"/>
-      <c r="B37" s="223">
+      <c r="B37" s="201">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C37" s="224"/>
-      <c r="D37" s="224"/>
-      <c r="E37" s="224"/>
-      <c r="F37" s="224"/>
-      <c r="G37" s="224"/>
-      <c r="H37" s="224"/>
-      <c r="I37" s="224"/>
-      <c r="J37" s="224"/>
-      <c r="K37" s="224"/>
-      <c r="L37" s="225"/>
+      <c r="C37" s="202"/>
+      <c r="D37" s="202"/>
+      <c r="E37" s="202"/>
+      <c r="F37" s="202"/>
+      <c r="G37" s="202"/>
+      <c r="H37" s="202"/>
+      <c r="I37" s="202"/>
+      <c r="J37" s="202"/>
+      <c r="K37" s="202"/>
+      <c r="L37" s="203"/>
       <c r="M37" s="9"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="4"/>
-      <c r="B38" s="223">
+      <c r="B38" s="201">
         <v>1.2</v>
       </c>
-      <c r="C38" s="224"/>
-      <c r="D38" s="224"/>
-      <c r="E38" s="224"/>
-      <c r="F38" s="224"/>
-      <c r="G38" s="224"/>
-      <c r="H38" s="224"/>
-      <c r="I38" s="224"/>
-      <c r="J38" s="224"/>
-      <c r="K38" s="224"/>
-      <c r="L38" s="225"/>
+      <c r="C38" s="202"/>
+      <c r="D38" s="202"/>
+      <c r="E38" s="202"/>
+      <c r="F38" s="202"/>
+      <c r="G38" s="202"/>
+      <c r="H38" s="202"/>
+      <c r="I38" s="202"/>
+      <c r="J38" s="202"/>
+      <c r="K38" s="202"/>
+      <c r="L38" s="203"/>
       <c r="M38" s="9"/>
     </row>
-    <row r="39" spans="1:13" ht="15" thickBot="1">
+    <row r="39" spans="1:13" ht="15.75" thickBot="1">
       <c r="A39" s="4"/>
-      <c r="B39" s="220">
+      <c r="B39" s="198">
         <v>1.3</v>
       </c>
-      <c r="C39" s="221"/>
-      <c r="D39" s="221"/>
-      <c r="E39" s="221"/>
-      <c r="F39" s="221"/>
-      <c r="G39" s="221"/>
-      <c r="H39" s="221"/>
-      <c r="I39" s="221"/>
-      <c r="J39" s="221"/>
-      <c r="K39" s="221"/>
-      <c r="L39" s="222"/>
+      <c r="C39" s="199"/>
+      <c r="D39" s="199"/>
+      <c r="E39" s="199"/>
+      <c r="F39" s="199"/>
+      <c r="G39" s="199"/>
+      <c r="H39" s="199"/>
+      <c r="I39" s="199"/>
+      <c r="J39" s="199"/>
+      <c r="K39" s="199"/>
+      <c r="L39" s="200"/>
       <c r="M39" s="9"/>
     </row>
     <row r="40" spans="1:13">
@@ -13769,6 +13775,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="K36:L36"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="E39:G39"/>
     <mergeCell ref="H39:J39"/>
@@ -13781,22 +13800,13 @@
     <mergeCell ref="E38:G38"/>
     <mergeCell ref="H38:J38"/>
     <mergeCell ref="K38:L38"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="B34:L34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <headerFooter differentOddEven="1">
+    <oddFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</oddFooter>
+    <evenFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</evenFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -13813,26 +13823,26 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="137" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.54296875" style="137" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" style="137"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.453125" customWidth="1"/>
-    <col min="8" max="8" width="18.36328125" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" customWidth="1"/>
-    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.26953125" customWidth="1"/>
-    <col min="25" max="25" width="9.26953125" style="137"/>
+    <col min="1" max="1" width="16.140625" style="137" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="137" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="137"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" style="137"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -13844,21 +13854,21 @@
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
-      <c r="E2" s="303" t="s">
+      <c r="E2" s="291" t="s">
         <v>306</v>
       </c>
-      <c r="F2" s="303"/>
-      <c r="G2" s="303"/>
-      <c r="H2" s="303"/>
-      <c r="I2" s="303"/>
-      <c r="J2" s="303"/>
-      <c r="K2" s="303"/>
-      <c r="L2" s="303"/>
-      <c r="M2" s="303"/>
-      <c r="N2" s="303"/>
-      <c r="O2" s="303"/>
-      <c r="P2" s="303"/>
-      <c r="Q2" s="303"/>
+      <c r="F2" s="291"/>
+      <c r="G2" s="291"/>
+      <c r="H2" s="291"/>
+      <c r="I2" s="291"/>
+      <c r="J2" s="291"/>
+      <c r="K2" s="291"/>
+      <c r="L2" s="291"/>
+      <c r="M2" s="291"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
+      <c r="P2" s="291"/>
+      <c r="Q2" s="291"/>
       <c r="S2" s="125"/>
       <c r="T2" s="125"/>
       <c r="U2" s="125"/>
@@ -13875,37 +13885,37 @@
       <c r="C3" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="307" t="s">
+      <c r="E3" s="297" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="305"/>
-      <c r="G3" s="305" t="s">
+      <c r="F3" s="294"/>
+      <c r="G3" s="294" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="305"/>
-      <c r="I3" s="305" t="s">
+      <c r="H3" s="294"/>
+      <c r="I3" s="294" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="305"/>
+      <c r="J3" s="294"/>
       <c r="K3" s="151"/>
-      <c r="L3" s="308" t="s">
+      <c r="L3" s="298" t="s">
         <v>296</v>
       </c>
-      <c r="M3" s="309"/>
-      <c r="N3" s="309"/>
-      <c r="O3" s="310"/>
-      <c r="P3" s="305" t="s">
+      <c r="M3" s="299"/>
+      <c r="N3" s="299"/>
+      <c r="O3" s="300"/>
+      <c r="P3" s="294" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="306"/>
-      <c r="S3" s="330" t="s">
+      <c r="Q3" s="295"/>
+      <c r="S3" s="327" t="s">
         <v>54</v>
       </c>
-      <c r="T3" s="331"/>
-      <c r="U3" s="318"/>
-      <c r="V3" s="319"/>
-      <c r="W3" s="319"/>
-      <c r="X3" s="320"/>
+      <c r="T3" s="328"/>
+      <c r="U3" s="323"/>
+      <c r="V3" s="324"/>
+      <c r="W3" s="324"/>
+      <c r="X3" s="325"/>
       <c r="Y3" s="146"/>
     </row>
     <row r="4" spans="1:25">
@@ -13957,14 +13967,14 @@
       <c r="Q4" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="332" t="s">
+      <c r="S4" s="329" t="s">
         <v>53</v>
       </c>
-      <c r="T4" s="333"/>
-      <c r="U4" s="318"/>
-      <c r="V4" s="319"/>
-      <c r="W4" s="319"/>
-      <c r="X4" s="320"/>
+      <c r="T4" s="330"/>
+      <c r="U4" s="323"/>
+      <c r="V4" s="324"/>
+      <c r="W4" s="324"/>
+      <c r="X4" s="325"/>
       <c r="Y4" s="146"/>
     </row>
     <row r="5" spans="1:25">
@@ -14019,14 +14029,14 @@
       <c r="Q5" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="S5" s="330" t="s">
+      <c r="S5" s="327" t="s">
         <v>42</v>
       </c>
-      <c r="T5" s="331"/>
-      <c r="U5" s="318"/>
-      <c r="V5" s="319"/>
-      <c r="W5" s="319"/>
-      <c r="X5" s="320"/>
+      <c r="T5" s="328"/>
+      <c r="U5" s="323"/>
+      <c r="V5" s="324"/>
+      <c r="W5" s="324"/>
+      <c r="X5" s="325"/>
       <c r="Y5" s="146"/>
     </row>
     <row r="6" spans="1:25">
@@ -14081,17 +14091,17 @@
       <c r="Q6" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="S6" s="332" t="s">
+      <c r="S6" s="329" t="s">
         <v>71</v>
       </c>
-      <c r="T6" s="333"/>
-      <c r="U6" s="318" t="str">
+      <c r="T6" s="330"/>
+      <c r="U6" s="323" t="str">
         <f>S4048_2_FW</f>
         <v>fw: 9.11(0.0P2)</v>
       </c>
-      <c r="V6" s="319"/>
-      <c r="W6" s="319"/>
-      <c r="X6" s="320"/>
+      <c r="V6" s="324"/>
+      <c r="W6" s="324"/>
+      <c r="X6" s="325"/>
       <c r="Y6" s="146"/>
     </row>
     <row r="7" spans="1:25">
@@ -14199,16 +14209,16 @@
       <c r="Q8" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="S8" s="315" t="s">
+      <c r="S8" s="320" t="s">
         <v>167</v>
       </c>
-      <c r="T8" s="316"/>
-      <c r="U8" s="317"/>
-      <c r="V8" s="327" t="s">
+      <c r="T8" s="321"/>
+      <c r="U8" s="322"/>
+      <c r="V8" s="331" t="s">
         <v>287</v>
       </c>
-      <c r="W8" s="328"/>
-      <c r="X8" s="329"/>
+      <c r="W8" s="332"/>
+      <c r="X8" s="333"/>
       <c r="Y8" s="139"/>
     </row>
     <row r="9" spans="1:25">
@@ -14268,9 +14278,9 @@
       </c>
       <c r="T9" s="335"/>
       <c r="U9" s="336"/>
-      <c r="V9" s="318"/>
-      <c r="W9" s="319"/>
-      <c r="X9" s="320"/>
+      <c r="V9" s="323"/>
+      <c r="W9" s="324"/>
+      <c r="X9" s="325"/>
       <c r="Y9" s="146"/>
     </row>
     <row r="10" spans="1:25">
@@ -14330,11 +14340,11 @@
       </c>
       <c r="T10" s="338"/>
       <c r="U10" s="339"/>
-      <c r="V10" s="318">
+      <c r="V10" s="323">
         <v>20480</v>
       </c>
-      <c r="W10" s="319"/>
-      <c r="X10" s="320"/>
+      <c r="W10" s="324"/>
+      <c r="X10" s="325"/>
       <c r="Y10" s="146"/>
     </row>
     <row r="11" spans="1:25">
@@ -14423,14 +14433,14 @@
       <c r="O12" s="130"/>
       <c r="P12" s="48"/>
       <c r="Q12" s="61"/>
-      <c r="S12" s="315" t="s">
+      <c r="S12" s="320" t="s">
         <v>59</v>
       </c>
-      <c r="T12" s="316"/>
-      <c r="U12" s="317"/>
-      <c r="V12" s="318"/>
-      <c r="W12" s="319"/>
-      <c r="X12" s="320"/>
+      <c r="T12" s="321"/>
+      <c r="U12" s="322"/>
+      <c r="V12" s="323"/>
+      <c r="W12" s="324"/>
+      <c r="X12" s="325"/>
       <c r="Y12" s="146"/>
     </row>
     <row r="13" spans="1:25">
@@ -14465,24 +14475,24 @@
       <c r="O13" s="130"/>
       <c r="P13" s="48"/>
       <c r="Q13" s="61"/>
-      <c r="S13" s="321" t="s">
+      <c r="S13" s="317" t="s">
         <v>60</v>
       </c>
-      <c r="T13" s="322"/>
-      <c r="U13" s="323"/>
-      <c r="V13" s="327">
+      <c r="T13" s="318"/>
+      <c r="U13" s="319"/>
+      <c r="V13" s="331">
         <f>VLTDOMAIN</f>
         <v>1</v>
       </c>
-      <c r="W13" s="328"/>
-      <c r="X13" s="329"/>
+      <c r="W13" s="332"/>
+      <c r="X13" s="333"/>
       <c r="Y13" s="139"/>
     </row>
     <row r="14" spans="1:25">
-      <c r="A14" s="307" t="s">
+      <c r="A14" s="297" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="306"/>
+      <c r="B14" s="295"/>
       <c r="E14" s="36" t="s">
         <v>237</v>
       </c>
@@ -14504,16 +14514,16 @@
       <c r="O14" s="130"/>
       <c r="P14" s="48"/>
       <c r="Q14" s="61"/>
-      <c r="S14" s="321" t="s">
+      <c r="S14" s="317" t="s">
         <v>166</v>
       </c>
-      <c r="T14" s="322"/>
-      <c r="U14" s="323"/>
-      <c r="V14" s="318">
+      <c r="T14" s="318"/>
+      <c r="U14" s="319"/>
+      <c r="V14" s="323">
         <v>2</v>
       </c>
-      <c r="W14" s="319"/>
-      <c r="X14" s="320"/>
+      <c r="W14" s="324"/>
+      <c r="X14" s="325"/>
       <c r="Y14" s="146"/>
     </row>
     <row r="15" spans="1:25">
@@ -14544,16 +14554,16 @@
       <c r="O15" s="130"/>
       <c r="P15" s="48"/>
       <c r="Q15" s="61"/>
-      <c r="S15" s="315" t="s">
+      <c r="S15" s="320" t="s">
         <v>67</v>
       </c>
-      <c r="T15" s="316"/>
-      <c r="U15" s="317"/>
-      <c r="V15" s="318">
+      <c r="T15" s="321"/>
+      <c r="U15" s="322"/>
+      <c r="V15" s="323">
         <v>1</v>
       </c>
-      <c r="W15" s="319"/>
-      <c r="X15" s="320"/>
+      <c r="W15" s="324"/>
+      <c r="X15" s="325"/>
       <c r="Y15" s="146"/>
     </row>
     <row r="16" spans="1:25">
@@ -14651,14 +14661,14 @@
       <c r="Q17" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="S17" s="311" t="s">
+      <c r="S17" s="301" t="s">
         <v>70</v>
       </c>
-      <c r="T17" s="312"/>
-      <c r="U17" s="312"/>
-      <c r="V17" s="312"/>
-      <c r="W17" s="312"/>
-      <c r="X17" s="313"/>
+      <c r="T17" s="302"/>
+      <c r="U17" s="302"/>
+      <c r="V17" s="302"/>
+      <c r="W17" s="302"/>
+      <c r="X17" s="303"/>
       <c r="Y17" s="140"/>
     </row>
     <row r="18" spans="1:25">
@@ -14707,12 +14717,12 @@
       <c r="Q18" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="S18" s="290"/>
-      <c r="T18" s="291"/>
-      <c r="U18" s="291"/>
-      <c r="V18" s="291"/>
-      <c r="W18" s="291"/>
-      <c r="X18" s="292"/>
+      <c r="S18" s="308"/>
+      <c r="T18" s="309"/>
+      <c r="U18" s="309"/>
+      <c r="V18" s="309"/>
+      <c r="W18" s="309"/>
+      <c r="X18" s="310"/>
       <c r="Y18" s="141"/>
     </row>
     <row r="19" spans="1:25">
@@ -14744,12 +14754,12 @@
       <c r="Q19" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="S19" s="293"/>
-      <c r="T19" s="294"/>
-      <c r="U19" s="294"/>
-      <c r="V19" s="294"/>
-      <c r="W19" s="294"/>
-      <c r="X19" s="295"/>
+      <c r="S19" s="311"/>
+      <c r="T19" s="312"/>
+      <c r="U19" s="312"/>
+      <c r="V19" s="312"/>
+      <c r="W19" s="312"/>
+      <c r="X19" s="313"/>
       <c r="Y19" s="141"/>
     </row>
     <row r="20" spans="1:25">
@@ -14781,12 +14791,12 @@
       <c r="Q20" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="S20" s="290"/>
-      <c r="T20" s="291"/>
-      <c r="U20" s="291"/>
-      <c r="V20" s="291"/>
-      <c r="W20" s="291"/>
-      <c r="X20" s="292"/>
+      <c r="S20" s="308"/>
+      <c r="T20" s="309"/>
+      <c r="U20" s="309"/>
+      <c r="V20" s="309"/>
+      <c r="W20" s="309"/>
+      <c r="X20" s="310"/>
       <c r="Y20" s="141"/>
     </row>
     <row r="21" spans="1:25">
@@ -14816,12 +14826,12 @@
       <c r="Q21" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="S21" s="293"/>
-      <c r="T21" s="294"/>
-      <c r="U21" s="294"/>
-      <c r="V21" s="294"/>
-      <c r="W21" s="294"/>
-      <c r="X21" s="295"/>
+      <c r="S21" s="311"/>
+      <c r="T21" s="312"/>
+      <c r="U21" s="312"/>
+      <c r="V21" s="312"/>
+      <c r="W21" s="312"/>
+      <c r="X21" s="313"/>
       <c r="Y21" s="141"/>
     </row>
     <row r="22" spans="1:25">
@@ -15167,9 +15177,9 @@
       </c>
     </row>
     <row r="32" spans="1:25">
-      <c r="A32" s="302"/>
-      <c r="B32" s="302"/>
-      <c r="C32" s="302"/>
+      <c r="A32" s="290"/>
+      <c r="B32" s="290"/>
+      <c r="C32" s="290"/>
       <c r="E32" s="36" t="s">
         <v>255</v>
       </c>
@@ -15212,9 +15222,9 @@
       </c>
     </row>
     <row r="33" spans="1:17">
-      <c r="A33" s="302"/>
-      <c r="B33" s="302"/>
-      <c r="C33" s="302"/>
+      <c r="A33" s="290"/>
+      <c r="B33" s="290"/>
+      <c r="C33" s="290"/>
       <c r="E33" s="36" t="s">
         <v>256</v>
       </c>
@@ -15257,9 +15267,9 @@
       </c>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="302"/>
-      <c r="B34" s="302"/>
-      <c r="C34" s="302"/>
+      <c r="A34" s="290"/>
+      <c r="B34" s="290"/>
+      <c r="C34" s="290"/>
       <c r="E34" s="36" t="s">
         <v>257</v>
       </c>
@@ -15344,10 +15354,10 @@
       </c>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="314" t="s">
+      <c r="A36" s="326" t="s">
         <v>399</v>
       </c>
-      <c r="B36" s="314"/>
+      <c r="B36" s="326"/>
       <c r="E36" s="36" t="s">
         <v>259</v>
       </c>
@@ -15371,8 +15381,8 @@
       <c r="Q36" s="61"/>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="314"/>
-      <c r="B37" s="314"/>
+      <c r="A37" s="326"/>
+      <c r="B37" s="326"/>
       <c r="E37" s="36" t="s">
         <v>260</v>
       </c>
@@ -16326,6 +16336,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="S18:X18"/>
+    <mergeCell ref="S19:X19"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="S17:X17"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="E2:Q2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="P3:Q3"/>
     <mergeCell ref="A32:C34"/>
     <mergeCell ref="S20:X20"/>
     <mergeCell ref="S21:X21"/>
@@ -16342,28 +16374,6 @@
     <mergeCell ref="V9:X9"/>
     <mergeCell ref="S10:U10"/>
     <mergeCell ref="V10:X10"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="E2:Q2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="V12:X12"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="S18:X18"/>
-    <mergeCell ref="S19:X19"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="V14:X14"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="V15:X15"/>
-    <mergeCell ref="S17:X17"/>
   </mergeCells>
   <conditionalFormatting sqref="F53:F54">
     <cfRule type="expression" dxfId="26" priority="2" stopIfTrue="1">
@@ -16382,6 +16392,10 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <headerFooter differentOddEven="1">
+    <oddFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</oddFooter>
+    <evenFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</evenFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
   <tableParts count="4">
     <tablePart r:id="rId3"/>
@@ -16403,19 +16417,19 @@
       <selection activeCell="F31" sqref="F31:H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="1.54296875" style="66" customWidth="1"/>
-    <col min="2" max="4" width="15.7265625" style="66" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" style="66" customWidth="1"/>
-    <col min="6" max="7" width="15.7265625" style="66" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="66" customWidth="1"/>
+    <col min="1" max="1" width="1.5703125" style="66" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" style="66" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="66" customWidth="1"/>
+    <col min="6" max="7" width="15.7109375" style="66" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="66" customWidth="1"/>
     <col min="9" max="9" width="4" style="66" customWidth="1"/>
-    <col min="10" max="10" width="0.7265625" style="66" customWidth="1"/>
-    <col min="11" max="11" width="23.1796875" style="96" customWidth="1"/>
-    <col min="12" max="12" width="29.26953125" style="96" customWidth="1"/>
-    <col min="13" max="13" width="66.26953125" style="96" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="66"/>
+    <col min="10" max="10" width="0.7109375" style="66" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" style="96" customWidth="1"/>
+    <col min="12" max="12" width="29.28515625" style="96" customWidth="1"/>
+    <col min="13" max="13" width="66.28515625" style="96" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="66"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="71" customFormat="1" ht="4.5" customHeight="1">
@@ -16436,15 +16450,15 @@
     </row>
     <row r="2" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A2" s="72"/>
-      <c r="B2" s="259" t="s">
+      <c r="B2" s="226" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="255"/>
-      <c r="D2" s="255"/>
-      <c r="E2" s="255"/>
-      <c r="F2" s="255"/>
-      <c r="G2" s="255"/>
-      <c r="H2" s="256"/>
+      <c r="C2" s="227"/>
+      <c r="D2" s="227"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="227"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="228"/>
       <c r="I2" s="72"/>
       <c r="J2" s="72"/>
       <c r="K2" s="72"/>
@@ -16454,124 +16468,124 @@
     </row>
     <row r="3" spans="1:14" s="73" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="72"/>
-      <c r="B3" s="248" t="s">
+      <c r="B3" s="229" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="249"/>
-      <c r="D3" s="250"/>
-      <c r="E3" s="248" t="s">
+      <c r="C3" s="230"/>
+      <c r="D3" s="231"/>
+      <c r="E3" s="229" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="249"/>
-      <c r="G3" s="249"/>
-      <c r="H3" s="250"/>
+      <c r="F3" s="230"/>
+      <c r="G3" s="230"/>
+      <c r="H3" s="231"/>
       <c r="I3" s="72"/>
       <c r="J3" s="72"/>
-      <c r="K3" s="260" t="s">
+      <c r="K3" s="232" t="s">
         <v>142</v>
       </c>
-      <c r="L3" s="261"/>
-      <c r="M3" s="262"/>
+      <c r="L3" s="233"/>
+      <c r="M3" s="234"/>
       <c r="N3" s="72"/>
     </row>
     <row r="4" spans="1:14" s="73" customFormat="1" ht="20.25" customHeight="1">
       <c r="A4" s="72"/>
-      <c r="B4" s="245"/>
-      <c r="C4" s="246"/>
-      <c r="D4" s="247"/>
-      <c r="E4" s="229"/>
-      <c r="F4" s="230"/>
-      <c r="G4" s="230"/>
-      <c r="H4" s="231"/>
+      <c r="B4" s="235"/>
+      <c r="C4" s="236"/>
+      <c r="D4" s="237"/>
+      <c r="E4" s="238"/>
+      <c r="F4" s="239"/>
+      <c r="G4" s="239"/>
+      <c r="H4" s="240"/>
       <c r="I4" s="72"/>
       <c r="J4" s="72"/>
-      <c r="K4" s="263"/>
-      <c r="L4" s="264"/>
-      <c r="M4" s="265"/>
+      <c r="K4" s="241"/>
+      <c r="L4" s="242"/>
+      <c r="M4" s="243"/>
       <c r="N4" s="72"/>
     </row>
     <row r="5" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="72"/>
-      <c r="B5" s="248" t="s">
+      <c r="B5" s="229" t="s">
         <v>200</v>
       </c>
-      <c r="C5" s="249"/>
-      <c r="D5" s="249"/>
-      <c r="E5" s="248" t="s">
+      <c r="C5" s="230"/>
+      <c r="D5" s="230"/>
+      <c r="E5" s="229" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="249"/>
-      <c r="G5" s="249"/>
-      <c r="H5" s="250"/>
+      <c r="F5" s="230"/>
+      <c r="G5" s="230"/>
+      <c r="H5" s="231"/>
       <c r="I5" s="72"/>
       <c r="J5" s="74"/>
-      <c r="K5" s="266"/>
-      <c r="L5" s="267"/>
-      <c r="M5" s="268"/>
+      <c r="K5" s="244"/>
+      <c r="L5" s="245"/>
+      <c r="M5" s="246"/>
       <c r="N5" s="72"/>
     </row>
     <row r="6" spans="1:14" s="73" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="72"/>
-      <c r="B6" s="272"/>
-      <c r="C6" s="273"/>
-      <c r="D6" s="273"/>
-      <c r="E6" s="274"/>
-      <c r="F6" s="274"/>
-      <c r="G6" s="274"/>
-      <c r="H6" s="274"/>
+      <c r="B6" s="250"/>
+      <c r="C6" s="251"/>
+      <c r="D6" s="251"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="252"/>
+      <c r="G6" s="252"/>
+      <c r="H6" s="252"/>
       <c r="I6" s="72"/>
       <c r="J6" s="74"/>
-      <c r="K6" s="266"/>
-      <c r="L6" s="267"/>
-      <c r="M6" s="268"/>
+      <c r="K6" s="244"/>
+      <c r="L6" s="245"/>
+      <c r="M6" s="246"/>
       <c r="N6" s="72"/>
     </row>
     <row r="7" spans="1:14" s="73" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="72"/>
-      <c r="B7" s="275"/>
-      <c r="C7" s="275"/>
-      <c r="D7" s="275"/>
-      <c r="E7" s="276"/>
-      <c r="F7" s="276"/>
-      <c r="G7" s="276"/>
-      <c r="H7" s="276"/>
+      <c r="B7" s="253"/>
+      <c r="C7" s="253"/>
+      <c r="D7" s="253"/>
+      <c r="E7" s="254"/>
+      <c r="F7" s="254"/>
+      <c r="G7" s="254"/>
+      <c r="H7" s="254"/>
       <c r="I7" s="72"/>
       <c r="J7" s="72"/>
-      <c r="K7" s="266"/>
-      <c r="L7" s="267"/>
-      <c r="M7" s="268"/>
+      <c r="K7" s="244"/>
+      <c r="L7" s="245"/>
+      <c r="M7" s="246"/>
       <c r="N7" s="72"/>
     </row>
     <row r="8" spans="1:14" s="73" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="72"/>
-      <c r="B8" s="275"/>
-      <c r="C8" s="275"/>
-      <c r="D8" s="275"/>
-      <c r="E8" s="276"/>
-      <c r="F8" s="276"/>
-      <c r="G8" s="276"/>
-      <c r="H8" s="276"/>
+      <c r="B8" s="253"/>
+      <c r="C8" s="253"/>
+      <c r="D8" s="253"/>
+      <c r="E8" s="254"/>
+      <c r="F8" s="254"/>
+      <c r="G8" s="254"/>
+      <c r="H8" s="254"/>
       <c r="I8" s="72"/>
       <c r="J8" s="72"/>
-      <c r="K8" s="266"/>
-      <c r="L8" s="267"/>
-      <c r="M8" s="268"/>
+      <c r="K8" s="244"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="246"/>
       <c r="N8" s="72"/>
     </row>
     <row r="9" spans="1:14" s="73" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="72"/>
-      <c r="B9" s="277"/>
-      <c r="C9" s="277"/>
-      <c r="D9" s="277"/>
-      <c r="E9" s="253"/>
-      <c r="F9" s="253"/>
-      <c r="G9" s="253"/>
-      <c r="H9" s="253"/>
+      <c r="B9" s="255"/>
+      <c r="C9" s="255"/>
+      <c r="D9" s="255"/>
+      <c r="E9" s="256"/>
+      <c r="F9" s="256"/>
+      <c r="G9" s="256"/>
+      <c r="H9" s="256"/>
       <c r="I9" s="72"/>
       <c r="J9" s="72"/>
-      <c r="K9" s="266"/>
-      <c r="L9" s="267"/>
-      <c r="M9" s="268"/>
+      <c r="K9" s="244"/>
+      <c r="L9" s="245"/>
+      <c r="M9" s="246"/>
       <c r="N9" s="72"/>
     </row>
     <row r="10" spans="1:14" s="73" customFormat="1" ht="5.25" customHeight="1">
@@ -16585,47 +16599,47 @@
       <c r="H10" s="76"/>
       <c r="I10" s="72"/>
       <c r="J10" s="72"/>
-      <c r="K10" s="266"/>
-      <c r="L10" s="267"/>
-      <c r="M10" s="268"/>
+      <c r="K10" s="244"/>
+      <c r="L10" s="245"/>
+      <c r="M10" s="246"/>
       <c r="N10" s="72"/>
     </row>
     <row r="11" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="72"/>
-      <c r="B11" s="254" t="s">
+      <c r="B11" s="257" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="255"/>
-      <c r="D11" s="255"/>
-      <c r="E11" s="255"/>
-      <c r="F11" s="255"/>
-      <c r="G11" s="255"/>
-      <c r="H11" s="256"/>
+      <c r="C11" s="227"/>
+      <c r="D11" s="227"/>
+      <c r="E11" s="227"/>
+      <c r="F11" s="227"/>
+      <c r="G11" s="227"/>
+      <c r="H11" s="228"/>
       <c r="I11" s="72"/>
       <c r="J11" s="72"/>
-      <c r="K11" s="266"/>
-      <c r="L11" s="267"/>
-      <c r="M11" s="268"/>
+      <c r="K11" s="244"/>
+      <c r="L11" s="245"/>
+      <c r="M11" s="246"/>
       <c r="N11" s="72"/>
     </row>
     <row r="12" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="72"/>
       <c r="B12" s="77"/>
-      <c r="C12" s="248" t="s">
+      <c r="C12" s="229" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="249"/>
-      <c r="E12" s="249"/>
-      <c r="F12" s="248" t="s">
+      <c r="D12" s="230"/>
+      <c r="E12" s="230"/>
+      <c r="F12" s="229" t="s">
         <v>146</v>
       </c>
-      <c r="G12" s="249"/>
-      <c r="H12" s="250"/>
+      <c r="G12" s="230"/>
+      <c r="H12" s="231"/>
       <c r="I12" s="72"/>
       <c r="J12" s="72"/>
-      <c r="K12" s="266"/>
-      <c r="L12" s="267"/>
-      <c r="M12" s="268"/>
+      <c r="K12" s="244"/>
+      <c r="L12" s="245"/>
+      <c r="M12" s="246"/>
       <c r="N12" s="72"/>
     </row>
     <row r="13" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1">
@@ -16633,17 +16647,17 @@
       <c r="B13" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="229"/>
-      <c r="D13" s="230"/>
-      <c r="E13" s="231"/>
-      <c r="F13" s="245"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="247"/>
+      <c r="C13" s="238"/>
+      <c r="D13" s="239"/>
+      <c r="E13" s="240"/>
+      <c r="F13" s="235"/>
+      <c r="G13" s="236"/>
+      <c r="H13" s="237"/>
       <c r="I13" s="72"/>
       <c r="J13" s="72"/>
-      <c r="K13" s="266"/>
-      <c r="L13" s="267"/>
-      <c r="M13" s="268"/>
+      <c r="K13" s="244"/>
+      <c r="L13" s="245"/>
+      <c r="M13" s="246"/>
       <c r="N13" s="72"/>
     </row>
     <row r="14" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1">
@@ -16651,17 +16665,17 @@
       <c r="B14" s="79" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="229"/>
-      <c r="D14" s="230"/>
-      <c r="E14" s="231"/>
-      <c r="F14" s="245"/>
-      <c r="G14" s="246"/>
-      <c r="H14" s="247"/>
+      <c r="C14" s="238"/>
+      <c r="D14" s="239"/>
+      <c r="E14" s="240"/>
+      <c r="F14" s="235"/>
+      <c r="G14" s="236"/>
+      <c r="H14" s="237"/>
       <c r="I14" s="72"/>
       <c r="J14" s="80"/>
-      <c r="K14" s="266"/>
-      <c r="L14" s="267"/>
-      <c r="M14" s="268"/>
+      <c r="K14" s="244"/>
+      <c r="L14" s="245"/>
+      <c r="M14" s="246"/>
       <c r="N14" s="72"/>
     </row>
     <row r="15" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1">
@@ -16669,17 +16683,17 @@
       <c r="B15" s="79" t="s">
         <v>148</v>
       </c>
-      <c r="C15" s="229"/>
-      <c r="D15" s="230"/>
-      <c r="E15" s="231"/>
-      <c r="F15" s="245"/>
-      <c r="G15" s="246"/>
-      <c r="H15" s="247"/>
+      <c r="C15" s="238"/>
+      <c r="D15" s="239"/>
+      <c r="E15" s="240"/>
+      <c r="F15" s="235"/>
+      <c r="G15" s="236"/>
+      <c r="H15" s="237"/>
       <c r="I15" s="72"/>
       <c r="J15" s="72"/>
-      <c r="K15" s="266"/>
-      <c r="L15" s="267"/>
-      <c r="M15" s="268"/>
+      <c r="K15" s="244"/>
+      <c r="L15" s="245"/>
+      <c r="M15" s="246"/>
       <c r="N15" s="72"/>
     </row>
     <row r="16" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -16687,17 +16701,17 @@
       <c r="B16" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="C16" s="229"/>
-      <c r="D16" s="230"/>
-      <c r="E16" s="231"/>
-      <c r="F16" s="245"/>
-      <c r="G16" s="246"/>
-      <c r="H16" s="247"/>
+      <c r="C16" s="238"/>
+      <c r="D16" s="239"/>
+      <c r="E16" s="240"/>
+      <c r="F16" s="235"/>
+      <c r="G16" s="236"/>
+      <c r="H16" s="237"/>
       <c r="I16" s="72"/>
       <c r="J16" s="72"/>
-      <c r="K16" s="269"/>
-      <c r="L16" s="270"/>
-      <c r="M16" s="271"/>
+      <c r="K16" s="247"/>
+      <c r="L16" s="248"/>
+      <c r="M16" s="249"/>
       <c r="N16" s="72"/>
     </row>
     <row r="17" spans="1:14" s="73" customFormat="1" ht="3" customHeight="1">
@@ -16718,15 +16732,15 @@
     </row>
     <row r="18" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="72"/>
-      <c r="B18" s="254" t="s">
+      <c r="B18" s="257" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="257"/>
-      <c r="D18" s="257"/>
-      <c r="E18" s="257"/>
-      <c r="F18" s="257"/>
-      <c r="G18" s="257"/>
-      <c r="H18" s="258"/>
+      <c r="C18" s="258"/>
+      <c r="D18" s="258"/>
+      <c r="E18" s="258"/>
+      <c r="F18" s="258"/>
+      <c r="G18" s="258"/>
+      <c r="H18" s="259"/>
       <c r="I18" s="72"/>
       <c r="J18" s="72"/>
       <c r="K18" s="72"/>
@@ -16737,16 +16751,16 @@
     <row r="19" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="72"/>
       <c r="B19" s="81"/>
-      <c r="C19" s="248" t="s">
+      <c r="C19" s="229" t="s">
         <v>151</v>
       </c>
-      <c r="D19" s="249"/>
-      <c r="E19" s="249"/>
-      <c r="F19" s="248" t="s">
+      <c r="D19" s="230"/>
+      <c r="E19" s="230"/>
+      <c r="F19" s="229" t="s">
         <v>152</v>
       </c>
-      <c r="G19" s="249"/>
-      <c r="H19" s="250"/>
+      <c r="G19" s="230"/>
+      <c r="H19" s="231"/>
       <c r="I19" s="72"/>
       <c r="J19" s="72"/>
       <c r="K19" s="72"/>
@@ -16759,12 +16773,12 @@
       <c r="B20" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="229"/>
-      <c r="D20" s="230"/>
-      <c r="E20" s="231"/>
-      <c r="F20" s="245"/>
-      <c r="G20" s="246"/>
-      <c r="H20" s="247"/>
+      <c r="C20" s="238"/>
+      <c r="D20" s="239"/>
+      <c r="E20" s="240"/>
+      <c r="F20" s="235"/>
+      <c r="G20" s="236"/>
+      <c r="H20" s="237"/>
       <c r="I20" s="72"/>
       <c r="J20" s="72"/>
       <c r="K20" s="72"/>
@@ -16777,12 +16791,12 @@
       <c r="B21" s="78" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="229"/>
-      <c r="D21" s="230"/>
-      <c r="E21" s="231"/>
-      <c r="F21" s="245"/>
-      <c r="G21" s="246"/>
-      <c r="H21" s="247"/>
+      <c r="C21" s="238"/>
+      <c r="D21" s="239"/>
+      <c r="E21" s="240"/>
+      <c r="F21" s="235"/>
+      <c r="G21" s="236"/>
+      <c r="H21" s="237"/>
       <c r="I21" s="72"/>
       <c r="J21" s="72"/>
       <c r="K21" s="72"/>
@@ -16795,12 +16809,12 @@
       <c r="B22" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C22" s="229"/>
-      <c r="D22" s="230"/>
-      <c r="E22" s="231"/>
-      <c r="F22" s="245"/>
-      <c r="G22" s="246"/>
-      <c r="H22" s="247"/>
+      <c r="C22" s="238"/>
+      <c r="D22" s="239"/>
+      <c r="E22" s="240"/>
+      <c r="F22" s="235"/>
+      <c r="G22" s="236"/>
+      <c r="H22" s="237"/>
       <c r="I22" s="72"/>
       <c r="J22" s="72"/>
       <c r="K22" s="72"/>
@@ -16813,12 +16827,12 @@
       <c r="B23" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="229"/>
-      <c r="D23" s="230"/>
-      <c r="E23" s="231"/>
-      <c r="F23" s="245"/>
-      <c r="G23" s="246"/>
-      <c r="H23" s="247"/>
+      <c r="C23" s="238"/>
+      <c r="D23" s="239"/>
+      <c r="E23" s="240"/>
+      <c r="F23" s="235"/>
+      <c r="G23" s="236"/>
+      <c r="H23" s="237"/>
       <c r="I23" s="72"/>
       <c r="J23" s="72"/>
       <c r="K23" s="72"/>
@@ -16829,16 +16843,16 @@
     <row r="24" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A24" s="72"/>
       <c r="B24" s="82"/>
-      <c r="C24" s="248" t="s">
+      <c r="C24" s="229" t="s">
         <v>154</v>
       </c>
-      <c r="D24" s="249"/>
-      <c r="E24" s="249"/>
-      <c r="F24" s="248" t="s">
+      <c r="D24" s="230"/>
+      <c r="E24" s="230"/>
+      <c r="F24" s="229" t="s">
         <v>155</v>
       </c>
-      <c r="G24" s="249"/>
-      <c r="H24" s="250"/>
+      <c r="G24" s="230"/>
+      <c r="H24" s="231"/>
       <c r="I24" s="72"/>
       <c r="J24" s="72"/>
       <c r="K24" s="72"/>
@@ -16851,12 +16865,12 @@
       <c r="B25" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="229"/>
-      <c r="D25" s="230"/>
-      <c r="E25" s="231"/>
-      <c r="F25" s="245"/>
-      <c r="G25" s="246"/>
-      <c r="H25" s="247"/>
+      <c r="C25" s="238"/>
+      <c r="D25" s="239"/>
+      <c r="E25" s="240"/>
+      <c r="F25" s="235"/>
+      <c r="G25" s="236"/>
+      <c r="H25" s="237"/>
       <c r="I25" s="72"/>
       <c r="J25" s="72"/>
       <c r="K25" s="83" t="s">
@@ -16871,12 +16885,12 @@
       <c r="B26" s="78" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="229"/>
-      <c r="D26" s="230"/>
-      <c r="E26" s="231"/>
-      <c r="F26" s="245"/>
-      <c r="G26" s="246"/>
-      <c r="H26" s="247"/>
+      <c r="C26" s="238"/>
+      <c r="D26" s="239"/>
+      <c r="E26" s="240"/>
+      <c r="F26" s="235"/>
+      <c r="G26" s="236"/>
+      <c r="H26" s="237"/>
       <c r="I26" s="72"/>
       <c r="J26" s="72"/>
       <c r="K26" s="85" t="s">
@@ -16891,12 +16905,12 @@
       <c r="B27" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C27" s="229"/>
-      <c r="D27" s="230"/>
-      <c r="E27" s="231"/>
-      <c r="F27" s="245"/>
-      <c r="G27" s="246"/>
-      <c r="H27" s="247"/>
+      <c r="C27" s="238"/>
+      <c r="D27" s="239"/>
+      <c r="E27" s="240"/>
+      <c r="F27" s="235"/>
+      <c r="G27" s="236"/>
+      <c r="H27" s="237"/>
       <c r="I27" s="72"/>
       <c r="J27" s="72"/>
       <c r="K27" s="85" t="s">
@@ -16911,12 +16925,12 @@
       <c r="B28" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="C28" s="229"/>
-      <c r="D28" s="230"/>
-      <c r="E28" s="231"/>
-      <c r="F28" s="245"/>
-      <c r="G28" s="246"/>
-      <c r="H28" s="247"/>
+      <c r="C28" s="238"/>
+      <c r="D28" s="239"/>
+      <c r="E28" s="240"/>
+      <c r="F28" s="235"/>
+      <c r="G28" s="236"/>
+      <c r="H28" s="237"/>
       <c r="I28" s="72"/>
       <c r="J28" s="72"/>
       <c r="K28" s="87" t="s">
@@ -16931,9 +16945,9 @@
       <c r="B29" s="78" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="236"/>
-      <c r="D29" s="251"/>
-      <c r="E29" s="252"/>
+      <c r="C29" s="260"/>
+      <c r="D29" s="261"/>
+      <c r="E29" s="262"/>
       <c r="F29" s="64"/>
       <c r="G29" s="90"/>
       <c r="H29" s="90"/>
@@ -16947,16 +16961,16 @@
     <row r="30" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1">
       <c r="A30" s="72"/>
       <c r="B30" s="82"/>
-      <c r="C30" s="248" t="s">
+      <c r="C30" s="229" t="s">
         <v>161</v>
       </c>
-      <c r="D30" s="249"/>
-      <c r="E30" s="250"/>
-      <c r="F30" s="248" t="s">
+      <c r="D30" s="230"/>
+      <c r="E30" s="231"/>
+      <c r="F30" s="229" t="s">
         <v>201</v>
       </c>
-      <c r="G30" s="249"/>
-      <c r="H30" s="250"/>
+      <c r="G30" s="230"/>
+      <c r="H30" s="231"/>
       <c r="I30" s="72"/>
       <c r="J30" s="72"/>
       <c r="K30" s="91"/>
@@ -16969,12 +16983,12 @@
       <c r="B31" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="229"/>
-      <c r="D31" s="230"/>
-      <c r="E31" s="231"/>
-      <c r="F31" s="232"/>
-      <c r="G31" s="233"/>
-      <c r="H31" s="234"/>
+      <c r="C31" s="238"/>
+      <c r="D31" s="239"/>
+      <c r="E31" s="240"/>
+      <c r="F31" s="266"/>
+      <c r="G31" s="267"/>
+      <c r="H31" s="268"/>
       <c r="I31" s="92"/>
       <c r="J31" s="92"/>
       <c r="K31" s="69"/>
@@ -16987,12 +17001,12 @@
       <c r="B32" s="78" t="s">
         <v>153</v>
       </c>
-      <c r="C32" s="229"/>
-      <c r="D32" s="230"/>
-      <c r="E32" s="231"/>
-      <c r="F32" s="232"/>
-      <c r="G32" s="233"/>
-      <c r="H32" s="234"/>
+      <c r="C32" s="238"/>
+      <c r="D32" s="239"/>
+      <c r="E32" s="240"/>
+      <c r="F32" s="266"/>
+      <c r="G32" s="267"/>
+      <c r="H32" s="268"/>
       <c r="I32" s="92"/>
       <c r="J32" s="92"/>
       <c r="K32" s="69"/>
@@ -17005,12 +17019,12 @@
       <c r="B33" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="229"/>
-      <c r="D33" s="230"/>
-      <c r="E33" s="231"/>
-      <c r="F33" s="232"/>
-      <c r="G33" s="233"/>
-      <c r="H33" s="234"/>
+      <c r="C33" s="238"/>
+      <c r="D33" s="239"/>
+      <c r="E33" s="240"/>
+      <c r="F33" s="266"/>
+      <c r="G33" s="267"/>
+      <c r="H33" s="268"/>
       <c r="I33" s="92"/>
       <c r="J33" s="92"/>
       <c r="K33" s="69"/>
@@ -17023,12 +17037,12 @@
       <c r="B34" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="C34" s="229"/>
-      <c r="D34" s="230"/>
-      <c r="E34" s="231"/>
-      <c r="F34" s="235"/>
-      <c r="G34" s="233"/>
-      <c r="H34" s="234"/>
+      <c r="C34" s="238"/>
+      <c r="D34" s="239"/>
+      <c r="E34" s="240"/>
+      <c r="F34" s="269"/>
+      <c r="G34" s="267"/>
+      <c r="H34" s="268"/>
       <c r="I34" s="92"/>
       <c r="J34" s="92"/>
       <c r="K34" s="69"/>
@@ -17041,9 +17055,9 @@
       <c r="B35" s="79" t="s">
         <v>162</v>
       </c>
-      <c r="C35" s="236"/>
-      <c r="D35" s="237"/>
-      <c r="E35" s="238"/>
+      <c r="C35" s="260"/>
+      <c r="D35" s="270"/>
+      <c r="E35" s="271"/>
       <c r="F35" s="93"/>
       <c r="G35" s="93"/>
       <c r="H35" s="93"/>
@@ -17054,7 +17068,7 @@
       <c r="M35" s="69"/>
       <c r="N35" s="92"/>
     </row>
-    <row r="36" spans="1:14" ht="13" thickBot="1">
+    <row r="36" spans="1:14" ht="13.5" thickBot="1">
       <c r="A36" s="92"/>
       <c r="B36" s="93"/>
       <c r="C36" s="93"/>
@@ -17072,12 +17086,12 @@
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="92"/>
-      <c r="B37" s="239" t="s">
+      <c r="B37" s="272" t="s">
         <v>163</v>
       </c>
-      <c r="C37" s="240"/>
-      <c r="D37" s="240"/>
-      <c r="E37" s="241"/>
+      <c r="C37" s="273"/>
+      <c r="D37" s="273"/>
+      <c r="E37" s="274"/>
       <c r="F37" s="93"/>
       <c r="G37" s="93"/>
       <c r="H37" s="93"/>
@@ -17090,11 +17104,11 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="92"/>
-      <c r="B38" s="242" t="s">
+      <c r="B38" s="275" t="s">
         <v>164</v>
       </c>
-      <c r="C38" s="243"/>
-      <c r="D38" s="244"/>
+      <c r="C38" s="276"/>
+      <c r="D38" s="277"/>
       <c r="E38" s="94"/>
       <c r="F38" s="93"/>
       <c r="G38" s="93"/>
@@ -17106,13 +17120,13 @@
       <c r="M38" s="69"/>
       <c r="N38" s="92"/>
     </row>
-    <row r="39" spans="1:14" ht="13" thickBot="1">
+    <row r="39" spans="1:14" ht="13.5" thickBot="1">
       <c r="A39" s="92"/>
-      <c r="B39" s="226" t="s">
+      <c r="B39" s="263" t="s">
         <v>165</v>
       </c>
-      <c r="C39" s="227"/>
-      <c r="D39" s="228"/>
+      <c r="C39" s="264"/>
+      <c r="D39" s="265"/>
       <c r="E39" s="95"/>
       <c r="F39" s="93"/>
       <c r="G39" s="93"/>
@@ -17142,6 +17156,54 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="C19:E19"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -17158,54 +17220,6 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:D38"/>
   </mergeCells>
   <conditionalFormatting sqref="B4 E4">
     <cfRule type="expression" dxfId="169" priority="7">
@@ -17244,15 +17258,15 @@
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="0.97" header="0.5" footer="0.5"/>
   <pageSetup scale="75" pageOrder="overThenDown" orientation="portrait" blackAndWhite="1" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;LDell Inc. Confidential&amp;C&amp;A
+  <headerFooter differentOddEven="1" alignWithMargins="0">
+    <oddFooter>&amp;C&amp;A
 &amp;F&amp;RPage &amp;P
 &amp;T
-&amp;D</oddFooter>
-    <evenFooter>&amp;LDell Inc. Confidential&amp;C&amp;A
+&amp;D&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</oddFooter>
+    <evenFooter>&amp;C&amp;A
 &amp;F&amp;RPage &amp;P
 &amp;T
-&amp;D</evenFooter>
+&amp;D&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</evenFooter>
     <firstFooter>&amp;LDell Inc. Confidential&amp;C&amp;A
 &amp;F&amp;RPage &amp;P
 &amp;T
@@ -17274,17 +17288,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7265625" style="59" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" style="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="59" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" style="59" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="59" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7265625" style="59" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" style="59" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="46"/>
-    <col min="9" max="16384" width="9.1796875" style="33"/>
+    <col min="1" max="1" width="5.7109375" style="59" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="59" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="46"/>
+    <col min="9" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -17297,7 +17311,7 @@
       <c r="G1" s="42"/>
       <c r="H1" s="43"/>
     </row>
-    <row r="2" spans="1:8" ht="18.5">
+    <row r="2" spans="1:8" ht="18.75">
       <c r="A2" s="278" t="s">
         <v>43</v>
       </c>
@@ -17738,7 +17752,11 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <headerFooter differentOddEven="1">
+    <oddFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</oddFooter>
+    <evenFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</evenFooter>
+  </headerFooter>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -17757,13 +17775,17 @@
       <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.1796875" style="52"/>
+    <col min="1" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter differentOddEven="1">
+    <oddFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</oddFooter>
+    <evenFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</evenFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <oleObjects>
@@ -17774,15 +17796,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>336550</xdr:colOff>
+                <xdr:colOff>333375</xdr:colOff>
                 <xdr:row>45</xdr:row>
-                <xdr:rowOff>6350</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -17809,13 +17831,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="19" max="19" width="35.1796875" customWidth="1"/>
-    <col min="20" max="20" width="31.453125" customWidth="1"/>
-    <col min="21" max="21" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.36328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7265625" customWidth="1"/>
+    <col min="19" max="19" width="35.140625" customWidth="1"/>
+    <col min="20" max="20" width="31.42578125" customWidth="1"/>
+    <col min="21" max="21" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" customWidth="1"/>
     <col min="24" max="24" width="35" customWidth="1"/>
-    <col min="25" max="30" width="7.7265625" customWidth="1"/>
+    <col min="25" max="30" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="19:22" ht="30.75" customHeight="1">
@@ -17950,7 +17972,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="13" spans="19:22" ht="14.5">
+    <row r="13" spans="19:22" ht="15">
       <c r="S13" s="186" t="s">
         <v>548</v>
       </c>
@@ -18180,6 +18202,10 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter differentOddEven="1">
+    <oddFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</oddFooter>
+    <evenFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</evenFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
   <tableParts count="2">
     <tablePart r:id="rId3"/>
@@ -18199,37 +18225,37 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" customWidth="1"/>
-    <col min="2" max="2" width="35.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.26953125" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.54296875" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.1796875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="24.1796875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="22.1796875" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="22.1796875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9.1796875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="26" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="17.26953125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="15.453125" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="18.453125" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="21.453125" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="18.453125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="17.28515625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="18.42578125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="21.42578125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="18.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -18240,7 +18266,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:29" ht="19">
+    <row r="2" spans="1:29" ht="18.75">
       <c r="A2" s="287" t="s">
         <v>72</v>
       </c>
@@ -18250,7 +18276,7 @@
       <c r="E2" s="288"/>
       <c r="F2" s="289"/>
     </row>
-    <row r="3" spans="1:29" ht="15" thickBot="1">
+    <row r="3" spans="1:29" ht="15.75" thickBot="1">
       <c r="A3" s="4"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -18294,7 +18320,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15" thickBot="1">
+    <row r="4" spans="1:29" ht="15.75" thickBot="1">
       <c r="A4" s="4"/>
       <c r="B4" s="285" t="s">
         <v>78</v>
@@ -18529,7 +18555,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="15" thickBot="1">
+    <row r="10" spans="1:29" ht="15.75" thickBot="1">
       <c r="A10" s="4"/>
       <c r="B10" s="285" t="s">
         <v>187</v>
@@ -18610,7 +18636,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="15" thickBot="1">
+    <row r="14" spans="1:29" ht="15.75" thickBot="1">
       <c r="A14" s="4"/>
       <c r="B14" s="98" t="s">
         <v>182</v>
@@ -18800,7 +18826,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="15" thickBot="1">
+    <row r="27" spans="1:29" ht="15.75" thickBot="1">
       <c r="A27" s="4"/>
       <c r="B27" s="285" t="s">
         <v>93</v>
@@ -18843,7 +18869,7 @@
       <c r="E30" s="8"/>
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="1:29" ht="15" thickBot="1">
+    <row r="31" spans="1:29" ht="15.75" thickBot="1">
       <c r="A31" s="4"/>
       <c r="B31" s="285" t="s">
         <v>98</v>
@@ -18901,7 +18927,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="9"/>
     </row>
-    <row r="37" spans="1:6" ht="15" thickBot="1">
+    <row r="37" spans="1:6" ht="15.75" thickBot="1">
       <c r="A37" s="4"/>
       <c r="B37" s="285" t="s">
         <v>109</v>
@@ -18961,7 +18987,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="9"/>
     </row>
-    <row r="43" spans="1:6" ht="15" thickBot="1">
+    <row r="43" spans="1:6" ht="15.75" thickBot="1">
       <c r="A43" s="4"/>
       <c r="B43" s="285" t="s">
         <v>119</v>
@@ -18981,7 +19007,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="9"/>
     </row>
-    <row r="45" spans="1:6" ht="15" thickBot="1">
+    <row r="45" spans="1:6" ht="15.75" thickBot="1">
       <c r="A45" s="4"/>
       <c r="B45" s="112" t="s">
         <v>122</v>
@@ -19011,7 +19037,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="9"/>
     </row>
-    <row r="48" spans="1:6" ht="15" thickBot="1">
+    <row r="48" spans="1:6" ht="15.75" thickBot="1">
       <c r="A48" s="4"/>
       <c r="B48" s="116" t="s">
         <v>125</v>
@@ -19043,7 +19069,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="9"/>
     </row>
-    <row r="51" spans="1:6" ht="15" thickBot="1">
+    <row r="51" spans="1:6" ht="15.75" thickBot="1">
       <c r="A51" s="4"/>
       <c r="B51" s="112" t="s">
         <v>125</v>
@@ -19075,7 +19101,7 @@
       <c r="E53" s="8"/>
       <c r="F53" s="9"/>
     </row>
-    <row r="54" spans="1:6" ht="15" thickBot="1">
+    <row r="54" spans="1:6" ht="15.75" thickBot="1">
       <c r="A54" s="4"/>
       <c r="B54" s="116" t="s">
         <v>125</v>
@@ -19127,7 +19153,7 @@
       <c r="E58" s="8"/>
       <c r="F58" s="9"/>
     </row>
-    <row r="59" spans="1:6" ht="15" thickBot="1">
+    <row r="59" spans="1:6" ht="15.75" thickBot="1">
       <c r="A59" s="4"/>
       <c r="B59" s="118" t="s">
         <v>125</v>
@@ -19179,7 +19205,7 @@
       <c r="E63" s="8"/>
       <c r="F63" s="9"/>
     </row>
-    <row r="64" spans="1:6" ht="15" thickBot="1">
+    <row r="64" spans="1:6" ht="15.75" thickBot="1">
       <c r="A64" s="4"/>
       <c r="B64" s="119" t="s">
         <v>125</v>
@@ -19221,7 +19247,7 @@
       <c r="E67" s="8"/>
       <c r="F67" s="9"/>
     </row>
-    <row r="68" spans="1:6" ht="15" thickBot="1">
+    <row r="68" spans="1:6" ht="15.75" thickBot="1">
       <c r="A68" s="4"/>
       <c r="B68" s="112" t="s">
         <v>130</v>
@@ -19414,6 +19440,10 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <headerFooter differentOddEven="1">
+    <oddFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</oddFooter>
+    <evenFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</evenFooter>
+  </headerFooter>
   <tableParts count="12">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -19443,30 +19473,30 @@
       <selection pane="bottomLeft" activeCell="L4" sqref="L4:L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="2" width="19.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" customWidth="1"/>
-    <col min="6" max="7" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.7265625" customWidth="1"/>
-    <col min="12" max="12" width="17.453125" customWidth="1"/>
-    <col min="13" max="13" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="43.5">
+    <row r="1" spans="1:20" ht="45">
       <c r="A1" s="156" t="s">
         <v>501</v>
       </c>
@@ -19536,7 +19566,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" thickBot="1">
+    <row r="2" spans="1:20" ht="30.75" thickBot="1">
       <c r="A2" s="156" t="s">
         <v>565</v>
       </c>
@@ -19578,7 +19608,7 @@
       <c r="S2" s="156"/>
       <c r="T2" s="156"/>
     </row>
-    <row r="3" spans="1:20" ht="15" thickBot="1">
+    <row r="3" spans="1:20" ht="15.75" thickBot="1">
       <c r="A3" s="158" t="s">
         <v>471</v>
       </c>
@@ -19608,7 +19638,7 @@
       <c r="S3" s="166"/>
       <c r="T3" s="166"/>
     </row>
-    <row r="4" spans="1:20" ht="15" thickBot="1">
+    <row r="4" spans="1:20" ht="30.75" thickBot="1">
       <c r="A4" s="158" t="s">
         <v>473</v>
       </c>
@@ -19652,7 +19682,7 @@
       <c r="S4" s="166"/>
       <c r="T4" s="166"/>
     </row>
-    <row r="5" spans="1:20" ht="15" thickBot="1">
+    <row r="5" spans="1:20" ht="30.75" thickBot="1">
       <c r="A5" s="158" t="s">
         <v>472</v>
       </c>
@@ -19694,7 +19724,7 @@
       <c r="S5" s="166"/>
       <c r="T5" s="166"/>
     </row>
-    <row r="6" spans="1:20" ht="15" thickBot="1">
+    <row r="6" spans="1:20" ht="15.75" thickBot="1">
       <c r="A6" s="166" t="s">
         <v>456</v>
       </c>
@@ -19748,7 +19778,7 @@
       </c>
       <c r="T6" s="166"/>
     </row>
-    <row r="7" spans="1:20" ht="15" thickBot="1">
+    <row r="7" spans="1:20" ht="15.75" thickBot="1">
       <c r="A7" s="166" t="s">
         <v>457</v>
       </c>
@@ -19802,7 +19832,7 @@
       </c>
       <c r="T7" s="166"/>
     </row>
-    <row r="8" spans="1:20" ht="15" thickBot="1">
+    <row r="8" spans="1:20" ht="15.75" thickBot="1">
       <c r="A8" s="166" t="s">
         <v>467</v>
       </c>
@@ -19852,7 +19882,7 @@
       </c>
       <c r="T8" s="166"/>
     </row>
-    <row r="9" spans="1:20" ht="15" thickBot="1">
+    <row r="9" spans="1:20" ht="15.75" thickBot="1">
       <c r="A9" s="166" t="s">
         <v>460</v>
       </c>
@@ -19906,7 +19936,7 @@
       </c>
       <c r="T9" s="166"/>
     </row>
-    <row r="10" spans="1:20" ht="15" thickBot="1">
+    <row r="10" spans="1:20" ht="15.75" thickBot="1">
       <c r="A10" s="166" t="s">
         <v>461</v>
       </c>
@@ -19960,7 +19990,7 @@
       </c>
       <c r="T10" s="166"/>
     </row>
-    <row r="11" spans="1:20" ht="15" thickBot="1">
+    <row r="11" spans="1:20" ht="15.75" thickBot="1">
       <c r="A11" s="166" t="s">
         <v>462</v>
       </c>
@@ -20014,7 +20044,7 @@
       </c>
       <c r="T11" s="166"/>
     </row>
-    <row r="12" spans="1:20" ht="15" thickBot="1">
+    <row r="12" spans="1:20" ht="15.75" thickBot="1">
       <c r="A12" s="166" t="s">
         <v>463</v>
       </c>
@@ -20066,7 +20096,7 @@
       </c>
       <c r="T12" s="166"/>
     </row>
-    <row r="13" spans="1:20" ht="15" thickBot="1">
+    <row r="13" spans="1:20" ht="15.75" thickBot="1">
       <c r="A13" s="166" t="s">
         <v>458</v>
       </c>
@@ -20118,7 +20148,7 @@
       </c>
       <c r="T13" s="166"/>
     </row>
-    <row r="14" spans="1:20" ht="15" thickBot="1">
+    <row r="14" spans="1:20" ht="15.75" thickBot="1">
       <c r="A14" s="166" t="s">
         <v>459</v>
       </c>
@@ -20170,7 +20200,7 @@
       </c>
       <c r="T14" s="166"/>
     </row>
-    <row r="15" spans="1:20" ht="15" thickBot="1">
+    <row r="15" spans="1:20" ht="15.75" thickBot="1">
       <c r="A15" s="170" t="s">
         <v>464</v>
       </c>
@@ -20224,7 +20254,7 @@
       </c>
       <c r="T15" s="166"/>
     </row>
-    <row r="16" spans="1:20" ht="15" thickBot="1">
+    <row r="16" spans="1:20" ht="15.75" thickBot="1">
       <c r="A16" s="170" t="s">
         <v>465</v>
       </c>
@@ -20278,7 +20308,7 @@
       </c>
       <c r="T16" s="166"/>
     </row>
-    <row r="17" spans="1:20" ht="15" thickBot="1">
+    <row r="17" spans="1:20" ht="15.75" thickBot="1">
       <c r="A17" s="170" t="s">
         <v>466</v>
       </c>
@@ -20332,7 +20362,7 @@
       </c>
       <c r="T17" s="166"/>
     </row>
-    <row r="18" spans="1:20" s="137" customFormat="1" ht="15" thickBot="1">
+    <row r="18" spans="1:20" s="137" customFormat="1" ht="15.75" thickBot="1">
       <c r="A18" s="195" t="s">
         <v>584</v>
       </c>
@@ -20958,10 +20988,10 @@
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="48" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;"museo sans for dell,Bold"&amp;KAAAAAA                 Dell - Internal Use - Confidential</oddFooter>
-    <evenFooter>&amp;L&amp;"museo sans for dell,Bold"&amp;KAAAAAA                 Dell - Internal Use - Confidential</evenFooter>
+  <pageSetup scale="41" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter differentOddEven="1">
+    <oddFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</oddFooter>
+    <evenFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</evenFooter>
     <firstFooter>&amp;L&amp;"museo sans for dell,Bold"&amp;KAAAAAA                 Dell - Internal Use - Confidential</firstFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
@@ -20980,43 +21010,43 @@
       <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7265625" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" customWidth="1"/>
-    <col min="15" max="15" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7265625" customWidth="1"/>
-    <col min="18" max="23" width="9.453125" customWidth="1"/>
-    <col min="24" max="26" width="5.7265625" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" customWidth="1"/>
+    <col min="18" max="23" width="9.42578125" customWidth="1"/>
+    <col min="24" max="26" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:24">
-      <c r="E2" s="303" t="s">
+      <c r="E2" s="291" t="s">
         <v>402</v>
       </c>
-      <c r="F2" s="303"/>
-      <c r="G2" s="303"/>
-      <c r="H2" s="303"/>
-      <c r="I2" s="303"/>
-      <c r="J2" s="303"/>
-      <c r="K2" s="303"/>
-      <c r="L2" s="303"/>
-      <c r="M2" s="303"/>
-      <c r="N2" s="303"/>
-      <c r="O2" s="303"/>
-      <c r="P2" s="303"/>
+      <c r="F2" s="291"/>
+      <c r="G2" s="291"/>
+      <c r="H2" s="291"/>
+      <c r="I2" s="291"/>
+      <c r="J2" s="291"/>
+      <c r="K2" s="291"/>
+      <c r="L2" s="291"/>
+      <c r="M2" s="291"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
+      <c r="P2" s="291"/>
       <c r="X2" s="137"/>
     </row>
     <row r="3" spans="1:24">
@@ -21027,36 +21057,36 @@
       <c r="C3" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="307" t="s">
+      <c r="E3" s="297" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="305"/>
-      <c r="G3" s="305" t="s">
+      <c r="F3" s="294"/>
+      <c r="G3" s="294" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="305"/>
-      <c r="I3" s="305" t="s">
+      <c r="H3" s="294"/>
+      <c r="I3" s="294" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="305"/>
-      <c r="K3" s="308" t="s">
+      <c r="J3" s="294"/>
+      <c r="K3" s="298" t="s">
         <v>296</v>
       </c>
-      <c r="L3" s="309"/>
-      <c r="M3" s="310"/>
+      <c r="L3" s="299"/>
+      <c r="M3" s="300"/>
       <c r="N3" s="150"/>
-      <c r="O3" s="305" t="s">
+      <c r="O3" s="294" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="306"/>
-      <c r="R3" s="304" t="s">
+      <c r="P3" s="295"/>
+      <c r="R3" s="292" t="s">
         <v>54</v>
       </c>
-      <c r="S3" s="304"/>
-      <c r="T3" s="298"/>
-      <c r="U3" s="298"/>
-      <c r="V3" s="298"/>
-      <c r="W3" s="298"/>
+      <c r="S3" s="292"/>
+      <c r="T3" s="293"/>
+      <c r="U3" s="293"/>
+      <c r="V3" s="293"/>
+      <c r="W3" s="293"/>
       <c r="X3" s="137"/>
     </row>
     <row r="4" spans="1:24">
@@ -21105,14 +21135,14 @@
       <c r="P4" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="R4" s="299" t="s">
+      <c r="R4" s="296" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="299"/>
-      <c r="T4" s="298"/>
-      <c r="U4" s="298"/>
-      <c r="V4" s="298"/>
-      <c r="W4" s="298"/>
+      <c r="S4" s="296"/>
+      <c r="T4" s="293"/>
+      <c r="U4" s="293"/>
+      <c r="V4" s="293"/>
+      <c r="W4" s="293"/>
       <c r="X4" s="137"/>
     </row>
     <row r="5" spans="1:24">
@@ -21162,14 +21192,14 @@
       <c r="P5" s="61" t="s">
         <v>587</v>
       </c>
-      <c r="R5" s="304" t="s">
+      <c r="R5" s="292" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="304"/>
-      <c r="T5" s="298"/>
-      <c r="U5" s="298"/>
-      <c r="V5" s="298"/>
-      <c r="W5" s="298"/>
+      <c r="S5" s="292"/>
+      <c r="T5" s="293"/>
+      <c r="U5" s="293"/>
+      <c r="V5" s="293"/>
+      <c r="W5" s="293"/>
       <c r="X5" s="137"/>
     </row>
     <row r="6" spans="1:24">
@@ -21219,17 +21249,17 @@
       <c r="P6" s="61" t="s">
         <v>587</v>
       </c>
-      <c r="R6" s="299" t="s">
+      <c r="R6" s="296" t="s">
         <v>71</v>
       </c>
-      <c r="S6" s="299"/>
-      <c r="T6" s="298" t="str">
+      <c r="S6" s="296"/>
+      <c r="T6" s="293" t="str">
         <f>S3048_FW</f>
         <v>fw: 9.11(0.0)</v>
       </c>
-      <c r="U6" s="298"/>
-      <c r="V6" s="298"/>
-      <c r="W6" s="298"/>
+      <c r="U6" s="293"/>
+      <c r="V6" s="293"/>
+      <c r="W6" s="293"/>
       <c r="X6" s="137"/>
     </row>
     <row r="7" spans="1:24">
@@ -21328,16 +21358,16 @@
       <c r="P8" s="61" t="s">
         <v>587</v>
       </c>
-      <c r="R8" s="296" t="s">
+      <c r="R8" s="304" t="s">
         <v>167</v>
       </c>
-      <c r="S8" s="296"/>
-      <c r="T8" s="296"/>
-      <c r="U8" s="297" t="s">
+      <c r="S8" s="304"/>
+      <c r="T8" s="304"/>
+      <c r="U8" s="305" t="s">
         <v>287</v>
       </c>
-      <c r="V8" s="297"/>
-      <c r="W8" s="297"/>
+      <c r="V8" s="305"/>
+      <c r="W8" s="305"/>
       <c r="X8" s="137"/>
     </row>
     <row r="9" spans="1:24">
@@ -21387,14 +21417,14 @@
       <c r="P9" s="61" t="s">
         <v>587</v>
       </c>
-      <c r="R9" s="300" t="s">
+      <c r="R9" s="306" t="s">
         <v>55</v>
       </c>
-      <c r="S9" s="300"/>
-      <c r="T9" s="300"/>
-      <c r="U9" s="298"/>
-      <c r="V9" s="298"/>
-      <c r="W9" s="298"/>
+      <c r="S9" s="306"/>
+      <c r="T9" s="306"/>
+      <c r="U9" s="293"/>
+      <c r="V9" s="293"/>
+      <c r="W9" s="293"/>
       <c r="X9" s="137"/>
     </row>
     <row r="10" spans="1:24">
@@ -21444,16 +21474,16 @@
       <c r="P10" s="61" t="s">
         <v>587</v>
       </c>
-      <c r="R10" s="301" t="s">
+      <c r="R10" s="307" t="s">
         <v>56</v>
       </c>
-      <c r="S10" s="301"/>
-      <c r="T10" s="301"/>
-      <c r="U10" s="298">
+      <c r="S10" s="307"/>
+      <c r="T10" s="307"/>
+      <c r="U10" s="293">
         <v>24576</v>
       </c>
-      <c r="V10" s="298"/>
-      <c r="W10" s="298"/>
+      <c r="V10" s="293"/>
+      <c r="W10" s="293"/>
       <c r="X10" s="137"/>
     </row>
     <row r="11" spans="1:24">
@@ -21542,16 +21572,16 @@
       <c r="P12" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R12" s="296" t="s">
+      <c r="R12" s="304" t="s">
         <v>58</v>
       </c>
-      <c r="S12" s="296"/>
-      <c r="T12" s="296"/>
-      <c r="U12" s="297" t="s">
+      <c r="S12" s="304"/>
+      <c r="T12" s="304"/>
+      <c r="U12" s="305" t="s">
         <v>288</v>
       </c>
-      <c r="V12" s="297"/>
-      <c r="W12" s="297"/>
+      <c r="V12" s="305"/>
+      <c r="W12" s="305"/>
       <c r="X12" s="137"/>
     </row>
     <row r="13" spans="1:24">
@@ -21593,10 +21623,10 @@
       <c r="X13" s="137"/>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="307" t="s">
+      <c r="A14" s="297" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="306"/>
+      <c r="B14" s="295"/>
       <c r="C14" s="34"/>
       <c r="E14" s="36" t="s">
         <v>326</v>
@@ -21623,14 +21653,14 @@
       <c r="P14" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R14" s="311" t="s">
+      <c r="R14" s="301" t="s">
         <v>70</v>
       </c>
-      <c r="S14" s="312"/>
-      <c r="T14" s="312"/>
-      <c r="U14" s="312"/>
-      <c r="V14" s="312"/>
-      <c r="W14" s="313"/>
+      <c r="S14" s="302"/>
+      <c r="T14" s="302"/>
+      <c r="U14" s="302"/>
+      <c r="V14" s="302"/>
+      <c r="W14" s="303"/>
       <c r="X14" s="137"/>
     </row>
     <row r="15" spans="1:24">
@@ -21668,12 +21698,12 @@
       <c r="P15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R15" s="290"/>
-      <c r="S15" s="291"/>
-      <c r="T15" s="291"/>
-      <c r="U15" s="291"/>
-      <c r="V15" s="291"/>
-      <c r="W15" s="292"/>
+      <c r="R15" s="308"/>
+      <c r="S15" s="309"/>
+      <c r="T15" s="309"/>
+      <c r="U15" s="309"/>
+      <c r="V15" s="309"/>
+      <c r="W15" s="310"/>
       <c r="X15" s="137"/>
     </row>
     <row r="16" spans="1:24">
@@ -21719,12 +21749,12 @@
       <c r="P16" s="61" t="s">
         <v>587</v>
       </c>
-      <c r="R16" s="293"/>
-      <c r="S16" s="294"/>
-      <c r="T16" s="294"/>
-      <c r="U16" s="294"/>
-      <c r="V16" s="294"/>
-      <c r="W16" s="295"/>
+      <c r="R16" s="311"/>
+      <c r="S16" s="312"/>
+      <c r="T16" s="312"/>
+      <c r="U16" s="312"/>
+      <c r="V16" s="312"/>
+      <c r="W16" s="313"/>
       <c r="X16" s="137"/>
     </row>
     <row r="17" spans="1:24">
@@ -21773,12 +21803,12 @@
       <c r="P17" s="61" t="s">
         <v>587</v>
       </c>
-      <c r="R17" s="290"/>
-      <c r="S17" s="291"/>
-      <c r="T17" s="291"/>
-      <c r="U17" s="291"/>
-      <c r="V17" s="291"/>
-      <c r="W17" s="292"/>
+      <c r="R17" s="308"/>
+      <c r="S17" s="309"/>
+      <c r="T17" s="309"/>
+      <c r="U17" s="309"/>
+      <c r="V17" s="309"/>
+      <c r="W17" s="310"/>
       <c r="X17" s="137"/>
     </row>
     <row r="18" spans="1:24">
@@ -21827,12 +21857,12 @@
       <c r="P18" s="61" t="s">
         <v>587</v>
       </c>
-      <c r="R18" s="293"/>
-      <c r="S18" s="294"/>
-      <c r="T18" s="294"/>
-      <c r="U18" s="294"/>
-      <c r="V18" s="294"/>
-      <c r="W18" s="295"/>
+      <c r="R18" s="311"/>
+      <c r="S18" s="312"/>
+      <c r="T18" s="312"/>
+      <c r="U18" s="312"/>
+      <c r="V18" s="312"/>
+      <c r="W18" s="313"/>
       <c r="X18" s="137"/>
     </row>
     <row r="19" spans="1:24">
@@ -22278,11 +22308,11 @@
       </c>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="302" t="s">
+      <c r="A31" s="290" t="s">
         <v>397</v>
       </c>
-      <c r="B31" s="302"/>
-      <c r="C31" s="302"/>
+      <c r="B31" s="290"/>
+      <c r="C31" s="290"/>
       <c r="E31" s="36" t="s">
         <v>343</v>
       </c>
@@ -22308,9 +22338,9 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="302"/>
-      <c r="B32" s="302"/>
-      <c r="C32" s="302"/>
+      <c r="A32" s="290"/>
+      <c r="B32" s="290"/>
+      <c r="C32" s="290"/>
       <c r="E32" s="36" t="s">
         <v>344</v>
       </c>
@@ -22347,10 +22377,10 @@
         <v>587</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="14.5" customHeight="1">
-      <c r="A33" s="302"/>
-      <c r="B33" s="302"/>
-      <c r="C33" s="302"/>
+    <row r="33" spans="1:16" ht="14.45" customHeight="1">
+      <c r="A33" s="290"/>
+      <c r="B33" s="290"/>
+      <c r="C33" s="290"/>
       <c r="E33" s="36" t="s">
         <v>345</v>
       </c>
@@ -22451,7 +22481,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="14.5" customHeight="1">
+    <row r="36" spans="1:16" ht="14.45" customHeight="1">
       <c r="E36" s="36" t="s">
         <v>348</v>
       </c>
@@ -23008,6 +23038,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="R15:W15"/>
+    <mergeCell ref="R16:W16"/>
+    <mergeCell ref="R17:W17"/>
+    <mergeCell ref="R18:W18"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="U12:W12"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="U10:W10"/>
     <mergeCell ref="A31:C33"/>
     <mergeCell ref="E2:P2"/>
     <mergeCell ref="R5:S5"/>
@@ -23024,21 +23069,6 @@
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="R14:W14"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="U12:W12"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="U9:W9"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="R15:W15"/>
-    <mergeCell ref="R16:W16"/>
-    <mergeCell ref="R17:W17"/>
-    <mergeCell ref="R18:W18"/>
-    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <conditionalFormatting sqref="F37:F43 F46:F48">
     <cfRule type="expression" dxfId="90" priority="6" stopIfTrue="1">
@@ -23080,6 +23110,10 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <headerFooter differentOddEven="1">
+    <oddFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</oddFooter>
+    <evenFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</evenFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
   <tableParts count="4">
     <tablePart r:id="rId3"/>
@@ -23102,79 +23136,79 @@
       <selection pane="bottomLeft" activeCell="X57" sqref="X57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" style="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7265625" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1796875" customWidth="1"/>
-    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7265625" customWidth="1"/>
-    <col min="20" max="26" width="9.26953125" customWidth="1"/>
-    <col min="27" max="27" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" customWidth="1"/>
+    <col min="20" max="26" width="9.28515625" customWidth="1"/>
+    <col min="27" max="27" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="21" customWidth="1"/>
-    <col min="29" max="29" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="5.7265625" customWidth="1"/>
+    <col min="29" max="29" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="E1" s="303" t="s">
+      <c r="E1" s="291" t="s">
         <v>402</v>
       </c>
-      <c r="F1" s="303"/>
-      <c r="G1" s="303"/>
-      <c r="H1" s="303"/>
-      <c r="I1" s="303"/>
-      <c r="J1" s="303"/>
-      <c r="K1" s="303"/>
-      <c r="L1" s="303"/>
-      <c r="M1" s="303"/>
-      <c r="N1" s="303"/>
-      <c r="O1" s="303"/>
-      <c r="P1" s="303"/>
-      <c r="Q1" s="303"/>
+      <c r="F1" s="291"/>
+      <c r="G1" s="291"/>
+      <c r="H1" s="291"/>
+      <c r="I1" s="291"/>
+      <c r="J1" s="291"/>
+      <c r="K1" s="291"/>
+      <c r="L1" s="291"/>
+      <c r="M1" s="291"/>
+      <c r="N1" s="291"/>
+      <c r="O1" s="291"/>
+      <c r="P1" s="291"/>
+      <c r="Q1" s="291"/>
     </row>
     <row r="2" spans="1:26">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
-      <c r="E2" s="307" t="s">
+      <c r="E2" s="297" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="305"/>
-      <c r="G2" s="305" t="s">
+      <c r="F2" s="294"/>
+      <c r="G2" s="294" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="305"/>
-      <c r="I2" s="305" t="s">
+      <c r="H2" s="294"/>
+      <c r="I2" s="294" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="305"/>
+      <c r="J2" s="294"/>
       <c r="K2" s="151"/>
-      <c r="L2" s="308" t="s">
+      <c r="L2" s="298" t="s">
         <v>296</v>
       </c>
-      <c r="M2" s="309"/>
-      <c r="N2" s="309"/>
-      <c r="O2" s="310"/>
-      <c r="P2" s="305" t="s">
+      <c r="M2" s="299"/>
+      <c r="N2" s="299"/>
+      <c r="O2" s="300"/>
+      <c r="P2" s="294" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="306"/>
+      <c r="Q2" s="295"/>
       <c r="Z2" s="137"/>
     </row>
     <row r="3" spans="1:26">
@@ -23224,14 +23258,14 @@
       <c r="Q3" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="T3" s="304" t="s">
+      <c r="T3" s="292" t="s">
         <v>54</v>
       </c>
-      <c r="U3" s="304"/>
-      <c r="V3" s="298"/>
-      <c r="W3" s="298"/>
-      <c r="X3" s="298"/>
-      <c r="Y3" s="298"/>
+      <c r="U3" s="292"/>
+      <c r="V3" s="293"/>
+      <c r="W3" s="293"/>
+      <c r="X3" s="293"/>
+      <c r="Y3" s="293"/>
       <c r="Z3" s="139"/>
     </row>
     <row r="4" spans="1:26">
@@ -23284,14 +23318,14 @@
       <c r="Q4" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T4" s="299" t="s">
+      <c r="T4" s="296" t="s">
         <v>53</v>
       </c>
-      <c r="U4" s="299"/>
-      <c r="V4" s="298"/>
-      <c r="W4" s="298"/>
-      <c r="X4" s="298"/>
-      <c r="Y4" s="298"/>
+      <c r="U4" s="296"/>
+      <c r="V4" s="293"/>
+      <c r="W4" s="293"/>
+      <c r="X4" s="293"/>
+      <c r="Y4" s="293"/>
       <c r="Z4" s="139"/>
     </row>
     <row r="5" spans="1:26">
@@ -23346,14 +23380,14 @@
       <c r="Q5" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T5" s="304" t="s">
+      <c r="T5" s="292" t="s">
         <v>42</v>
       </c>
-      <c r="U5" s="304"/>
-      <c r="V5" s="298"/>
-      <c r="W5" s="298"/>
-      <c r="X5" s="298"/>
-      <c r="Y5" s="298"/>
+      <c r="U5" s="292"/>
+      <c r="V5" s="293"/>
+      <c r="W5" s="293"/>
+      <c r="X5" s="293"/>
+      <c r="Y5" s="293"/>
       <c r="Z5" s="139"/>
     </row>
     <row r="6" spans="1:26">
@@ -23408,17 +23442,17 @@
       <c r="Q6" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T6" s="299" t="s">
+      <c r="T6" s="296" t="s">
         <v>71</v>
       </c>
-      <c r="U6" s="299"/>
-      <c r="V6" s="298" t="str">
+      <c r="U6" s="296"/>
+      <c r="V6" s="293" t="str">
         <f>S4048_1_FW</f>
         <v>fw: 9.11(0.0P2)</v>
       </c>
-      <c r="W6" s="298"/>
-      <c r="X6" s="298"/>
-      <c r="Y6" s="298"/>
+      <c r="W6" s="293"/>
+      <c r="X6" s="293"/>
+      <c r="Y6" s="293"/>
       <c r="Z6" s="139"/>
     </row>
     <row r="7" spans="1:26">
@@ -23527,16 +23561,16 @@
       <c r="Q8" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T8" s="296" t="s">
+      <c r="T8" s="304" t="s">
         <v>167</v>
       </c>
-      <c r="U8" s="296"/>
-      <c r="V8" s="296"/>
-      <c r="W8" s="297" t="s">
+      <c r="U8" s="304"/>
+      <c r="V8" s="304"/>
+      <c r="W8" s="305" t="s">
         <v>287</v>
       </c>
-      <c r="X8" s="297"/>
-      <c r="Y8" s="297"/>
+      <c r="X8" s="305"/>
+      <c r="Y8" s="305"/>
       <c r="Z8" s="139"/>
     </row>
     <row r="9" spans="1:26">
@@ -23591,14 +23625,14 @@
       <c r="Q9" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T9" s="300" t="s">
+      <c r="T9" s="306" t="s">
         <v>55</v>
       </c>
-      <c r="U9" s="300"/>
-      <c r="V9" s="300"/>
-      <c r="W9" s="298"/>
-      <c r="X9" s="298"/>
-      <c r="Y9" s="298"/>
+      <c r="U9" s="306"/>
+      <c r="V9" s="306"/>
+      <c r="W9" s="293"/>
+      <c r="X9" s="293"/>
+      <c r="Y9" s="293"/>
       <c r="Z9" s="139"/>
     </row>
     <row r="10" spans="1:26">
@@ -23653,16 +23687,16 @@
       <c r="Q10" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T10" s="301" t="s">
+      <c r="T10" s="307" t="s">
         <v>56</v>
       </c>
-      <c r="U10" s="301"/>
-      <c r="V10" s="301"/>
-      <c r="W10" s="298">
+      <c r="U10" s="307"/>
+      <c r="V10" s="307"/>
+      <c r="W10" s="293">
         <v>16384</v>
       </c>
-      <c r="X10" s="298"/>
-      <c r="Y10" s="298"/>
+      <c r="X10" s="293"/>
+      <c r="Y10" s="293"/>
       <c r="Z10" s="139"/>
     </row>
     <row r="11" spans="1:26">
@@ -23733,14 +23767,14 @@
       <c r="O12" s="130"/>
       <c r="P12" s="48"/>
       <c r="Q12" s="61"/>
-      <c r="T12" s="315" t="s">
+      <c r="T12" s="320" t="s">
         <v>59</v>
       </c>
-      <c r="U12" s="316"/>
-      <c r="V12" s="317"/>
-      <c r="W12" s="318"/>
-      <c r="X12" s="319"/>
-      <c r="Y12" s="320"/>
+      <c r="U12" s="321"/>
+      <c r="V12" s="322"/>
+      <c r="W12" s="323"/>
+      <c r="X12" s="324"/>
+      <c r="Y12" s="325"/>
       <c r="Z12" s="139"/>
     </row>
     <row r="13" spans="1:26">
@@ -23775,16 +23809,16 @@
       <c r="O13" s="130"/>
       <c r="P13" s="48"/>
       <c r="Q13" s="61"/>
-      <c r="T13" s="321" t="s">
+      <c r="T13" s="317" t="s">
         <v>60</v>
       </c>
-      <c r="U13" s="322"/>
-      <c r="V13" s="323"/>
-      <c r="W13" s="324">
+      <c r="U13" s="318"/>
+      <c r="V13" s="319"/>
+      <c r="W13" s="314">
         <v>1</v>
       </c>
-      <c r="X13" s="325"/>
-      <c r="Y13" s="326"/>
+      <c r="X13" s="315"/>
+      <c r="Y13" s="316"/>
       <c r="Z13" s="139"/>
     </row>
     <row r="14" spans="1:26">
@@ -23812,23 +23846,23 @@
       <c r="O14" s="130"/>
       <c r="P14" s="48"/>
       <c r="Q14" s="61"/>
-      <c r="T14" s="321" t="s">
+      <c r="T14" s="317" t="s">
         <v>166</v>
       </c>
-      <c r="U14" s="322"/>
-      <c r="V14" s="323"/>
-      <c r="W14" s="318">
+      <c r="U14" s="318"/>
+      <c r="V14" s="319"/>
+      <c r="W14" s="323">
         <v>1</v>
       </c>
-      <c r="X14" s="319"/>
-      <c r="Y14" s="320"/>
+      <c r="X14" s="324"/>
+      <c r="Y14" s="325"/>
       <c r="Z14" s="139"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" s="307" t="s">
+      <c r="A15" s="297" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="306"/>
+      <c r="B15" s="295"/>
       <c r="C15" s="36"/>
       <c r="E15" s="36" t="s">
         <v>239</v>
@@ -23870,16 +23904,16 @@
       <c r="Q15" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T15" s="315" t="s">
+      <c r="T15" s="320" t="s">
         <v>67</v>
       </c>
-      <c r="U15" s="316"/>
-      <c r="V15" s="317"/>
-      <c r="W15" s="318">
+      <c r="U15" s="321"/>
+      <c r="V15" s="322"/>
+      <c r="W15" s="323">
         <v>0</v>
       </c>
-      <c r="X15" s="319"/>
-      <c r="Y15" s="320"/>
+      <c r="X15" s="324"/>
+      <c r="Y15" s="325"/>
       <c r="Z15" s="139"/>
     </row>
     <row r="16" spans="1:26">
@@ -23980,14 +24014,14 @@
       <c r="Q17" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T17" s="311" t="s">
+      <c r="T17" s="301" t="s">
         <v>70</v>
       </c>
-      <c r="U17" s="312"/>
-      <c r="V17" s="312"/>
-      <c r="W17" s="312"/>
-      <c r="X17" s="312"/>
-      <c r="Y17" s="313"/>
+      <c r="U17" s="302"/>
+      <c r="V17" s="302"/>
+      <c r="W17" s="302"/>
+      <c r="X17" s="302"/>
+      <c r="Y17" s="303"/>
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="39">
@@ -24020,12 +24054,12 @@
       <c r="Q18" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="T18" s="290"/>
-      <c r="U18" s="291"/>
-      <c r="V18" s="291"/>
-      <c r="W18" s="291"/>
-      <c r="X18" s="291"/>
-      <c r="Y18" s="292"/>
+      <c r="T18" s="308"/>
+      <c r="U18" s="309"/>
+      <c r="V18" s="309"/>
+      <c r="W18" s="309"/>
+      <c r="X18" s="309"/>
+      <c r="Y18" s="310"/>
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="39">
@@ -24058,12 +24092,12 @@
       <c r="Q19" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="T19" s="293"/>
-      <c r="U19" s="294"/>
-      <c r="V19" s="294"/>
-      <c r="W19" s="294"/>
-      <c r="X19" s="294"/>
-      <c r="Y19" s="295"/>
+      <c r="T19" s="311"/>
+      <c r="U19" s="312"/>
+      <c r="V19" s="312"/>
+      <c r="W19" s="312"/>
+      <c r="X19" s="312"/>
+      <c r="Y19" s="313"/>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" s="39">
@@ -24092,12 +24126,12 @@
       <c r="Q20" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="T20" s="290"/>
-      <c r="U20" s="291"/>
-      <c r="V20" s="291"/>
-      <c r="W20" s="291"/>
-      <c r="X20" s="291"/>
-      <c r="Y20" s="292"/>
+      <c r="T20" s="308"/>
+      <c r="U20" s="309"/>
+      <c r="V20" s="309"/>
+      <c r="W20" s="309"/>
+      <c r="X20" s="309"/>
+      <c r="Y20" s="310"/>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="39">
@@ -24126,12 +24160,12 @@
       <c r="Q21" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="T21" s="293"/>
-      <c r="U21" s="294"/>
-      <c r="V21" s="294"/>
-      <c r="W21" s="294"/>
-      <c r="X21" s="294"/>
-      <c r="Y21" s="295"/>
+      <c r="T21" s="311"/>
+      <c r="U21" s="312"/>
+      <c r="V21" s="312"/>
+      <c r="W21" s="312"/>
+      <c r="X21" s="312"/>
+      <c r="Y21" s="313"/>
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="39">
@@ -24244,10 +24278,10 @@
       </c>
     </row>
     <row r="26" spans="1:25">
-      <c r="A26" s="314" t="s">
+      <c r="A26" s="326" t="s">
         <v>398</v>
       </c>
-      <c r="B26" s="314"/>
+      <c r="B26" s="326"/>
       <c r="C26" s="36"/>
       <c r="E26" s="36" t="s">
         <v>250</v>
@@ -24272,8 +24306,8 @@
       </c>
     </row>
     <row r="27" spans="1:25">
-      <c r="A27" s="314"/>
-      <c r="B27" s="314"/>
+      <c r="A27" s="326"/>
+      <c r="B27" s="326"/>
       <c r="C27" s="36"/>
       <c r="E27" s="36" t="s">
         <v>251</v>
@@ -24526,9 +24560,9 @@
       </c>
     </row>
     <row r="33" spans="1:17">
-      <c r="A33" s="302"/>
-      <c r="B33" s="302"/>
-      <c r="C33" s="302"/>
+      <c r="A33" s="290"/>
+      <c r="B33" s="290"/>
+      <c r="C33" s="290"/>
       <c r="E33" s="36" t="s">
         <v>257</v>
       </c>
@@ -24571,9 +24605,9 @@
       </c>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="302"/>
-      <c r="B34" s="302"/>
-      <c r="C34" s="302"/>
+      <c r="A34" s="290"/>
+      <c r="B34" s="290"/>
+      <c r="C34" s="290"/>
       <c r="E34" s="36" t="s">
         <v>258</v>
       </c>
@@ -24616,9 +24650,9 @@
       </c>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="302"/>
-      <c r="B35" s="302"/>
-      <c r="C35" s="302"/>
+      <c r="A35" s="290"/>
+      <c r="B35" s="290"/>
+      <c r="C35" s="290"/>
       <c r="E35" s="36" t="s">
         <v>259</v>
       </c>
@@ -25340,6 +25374,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="E1:Q1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="A26:B27"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="T15:V15"/>
+    <mergeCell ref="W15:Y15"/>
+    <mergeCell ref="T17:Y17"/>
+    <mergeCell ref="T18:Y18"/>
+    <mergeCell ref="W14:Y14"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="W8:Y8"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V6:Y6"/>
     <mergeCell ref="A33:C35"/>
     <mergeCell ref="T20:Y20"/>
     <mergeCell ref="T21:Y21"/>
@@ -25356,28 +25412,6 @@
     <mergeCell ref="W12:Y12"/>
     <mergeCell ref="W10:Y10"/>
     <mergeCell ref="T19:Y19"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="W8:Y8"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V6:Y6"/>
-    <mergeCell ref="T15:V15"/>
-    <mergeCell ref="W15:Y15"/>
-    <mergeCell ref="T17:Y17"/>
-    <mergeCell ref="T18:Y18"/>
-    <mergeCell ref="W14:Y14"/>
-    <mergeCell ref="T14:V14"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="E1:Q1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A26:B27"/>
-    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="F52:F53">
     <cfRule type="expression" dxfId="53" priority="2" stopIfTrue="1">
@@ -25396,6 +25430,10 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter differentOddEven="1">
+    <oddFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</oddFooter>
+    <evenFooter>&amp;L&amp;"arial,Regular"&amp;10&amp;KAAAAAA &amp;"Arial,Regular"Dell - Internal Use - Confidential - Customer Workproduct</evenFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
   <tableParts count="4">
     <tablePart r:id="rId3"/>
@@ -25521,18 +25559,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25552,6 +25590,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7243C670-E16E-4DBD-9932-9E3C368D5054}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42535616-3E13-4575-9B51-ECA7D821FF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -25564,12 +25610,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7243C670-E16E-4DBD-9932-9E3C368D5054}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>